<commit_message>
total is ok. but no keep format
</commit_message>
<xml_diff>
--- a/QueryReport/excelTemplate/Employee_template222_20200323.xlsx
+++ b/QueryReport/excelTemplate/Employee_template222_20200323.xlsx
@@ -342,8 +342,9 @@
     <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
     <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
     <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
+    <x:numFmt numFmtId="240" formatCode="yyyy-mm-dd"/>
   </x:numFmts>
-  <x:fonts count="40">
+  <x:fonts count="42">
     <x:font>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
@@ -383,6 +384,17 @@
       <x:name val="Microsoft YaHei"/>
       <x:family val="2"/>
       <x:charset val="134"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:color rgb="000000"/>
+    </x:font>
+    <x:font>
+      <x:name val="Microsoft YaHei"/>
+      <x:sz val="11"/>
+      <x:b/>
+      <x:color rgb="000000"/>
     </x:font>
     <x:font>
       <x:name val="Microsoft YaHei"/>
@@ -711,7 +723,7 @@
       <x:alignment vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="67">
+  <x:cellXfs count="70">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment vertical="center"/>
     </x:xf>
@@ -801,6 +813,9 @@
     <x:xf fontId="38" borderId="0" applyFont="1"/>
     <x:xf fontId="39" borderId="0" applyFont="1"/>
     <x:xf numFmtId="240" fontId="38" borderId="0" applyNumberFormat="1" applyFont="1"/>
+    <x:xf fontId="40" borderId="0" applyFont="1"/>
+    <x:xf fontId="41" borderId="0" applyFont="1"/>
+    <x:xf numFmtId="240" fontId="40" borderId="0" applyNumberFormat="1" applyFont="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,7 +836,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:pivotCacheDefinition xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" r:id="rId1" refreshOnLoad="1" refreshedBy="Administrator" refreshedDate="43913.642617129626" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="16" xr:uid="{CF51BC23-A1A6-4DE3-85A0-7D4C21EB6AB0}" mc:Ignorable="xr">
   <x:cacheSource type="worksheet">
-    <x:worksheetSource ref="B2:V53" sheet="Report"/>
+    <x:worksheetSource ref="B1:V52" sheet="Report"/>
   </x:cacheSource>
   <x:cacheFields count="23">
     <x:cacheField name="Contract Description" numFmtId="0">
@@ -1723,3382 +1738,3388 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1">
-      <x:c r="B1" s="61" t="str">
+      <x:c r="A1" s="67" t="str">
+        <x:v>_DATASTART</x:v>
+      </x:c>
+      <x:c r="B1" s="67" t="str">
         <x:v>Contract Description</x:v>
       </x:c>
-      <x:c r="C1" s="61" t="str">
+      <x:c r="C1" s="67" t="str">
         <x:v>Staff Number</x:v>
       </x:c>
-      <x:c r="D1" s="61" t="str">
+      <x:c r="D1" s="67" t="str">
         <x:v>ename</x:v>
       </x:c>
-      <x:c r="E1" s="61" t="str">
+      <x:c r="E1" s="67" t="str">
         <x:v>Zone Name</x:v>
       </x:c>
-      <x:c r="F1" s="61" t="str">
+      <x:c r="F1" s="67" t="str">
         <x:v>Rank Name</x:v>
       </x:c>
-      <x:c r="G1" s="61" t="str">
+      <x:c r="G1" s="67" t="str">
         <x:v>Postition Code</x:v>
       </x:c>
-      <x:c r="H1" s="61" t="str">
+      <x:c r="H1" s="67" t="str">
         <x:v>p name ok 3</x:v>
       </x:c>
-      <x:c r="I1" s="61" t="str">
+      <x:c r="I1" s="67" t="str">
         <x:v>Join Date</x:v>
       </x:c>
-      <x:c r="J1" s="61" t="str">
+      <x:c r="J1" s="67" t="str">
         <x:v>Year of Service</x:v>
       </x:c>
-      <x:c r="K1" s="61" t="str">
+      <x:c r="K1" s="67" t="str">
         <x:v>Annual Leave Class</x:v>
       </x:c>
-      <x:c r="L1" s="61" t="str">
+      <x:c r="L1" s="67" t="str">
         <x:v>~!</x:v>
       </x:c>
-      <x:c r="M1" s="61" t="str">
+      <x:c r="M1" s="67" t="str">
         <x:v>Employment Type</x:v>
       </x:c>
-      <x:c r="N1" s="61" t="str">
+      <x:c r="N1" s="67" t="str">
         <x:v>Basic Salary</x:v>
       </x:c>
-      <x:c r="O1" s="61" t="str">
+      <x:c r="O1" s="67" t="str">
         <x:v>Pay Scale Point</x:v>
       </x:c>
-      <x:c r="P1" s="61" t="str">
+      <x:c r="P1" s="67" t="str">
         <x:v>PayScale Scheme</x:v>
       </x:c>
-      <x:c r="Q1" s="61" t="str">
+      <x:c r="Q1" s="67" t="str">
         <x:v>Commence Date</x:v>
       </x:c>
-      <x:c r="R1" s="61" t="str">
+      <x:c r="R1" s="67" t="str">
         <x:v>Terminate Date</x:v>
       </x:c>
-      <x:c r="S1" s="61" t="str">
+      <x:c r="S1" s="67" t="str">
         <x:v>Staff Status</x:v>
       </x:c>
-      <x:c r="T1" s="61" t="str">
+      <x:c r="T1" s="67" t="str">
         <x:v>Part Time</x:v>
       </x:c>
-      <x:c r="U1" s="61" t="str">
+      <x:c r="U1" s="67" t="str">
         <x:v>SecurityGroupID</x:v>
       </x:c>
-      <x:c r="V1" s="61" t="str">
+      <x:c r="V1" s="67" t="str">
         <x:v>Securtiy Group</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
-      <x:c r="B2" s="61" t="str">
+      <x:c r="B2" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C2" s="61" t="str">
+      <x:c r="C2" s="67" t="str">
         <x:v>S30163</x:v>
       </x:c>
-      <x:c r="D2" s="61" t="str">
+      <x:c r="D2" s="67" t="str">
         <x:v>Wong Kam Tim</x:v>
       </x:c>
-      <x:c r="E2" s="61" t="str">
+      <x:c r="E2" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F2" s="61" t="str">
+      <x:c r="F2" s="67" t="str">
         <x:v>Assistant Manager 主管</x:v>
       </x:c>
-      <x:c r="G2" s="61" t="str">
+      <x:c r="G2" s="67" t="str">
         <x:v>IC</x:v>
       </x:c>
-      <x:c r="H2" s="61" t="str">
+      <x:c r="H2" s="67" t="str">
         <x:v>Unit Incharge</x:v>
       </x:c>
-      <x:c r="I2" s="63" t="d">
+      <x:c r="I2" s="69" t="d">
         <x:v>2010-03-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J2" s="61" t="n">
-        <x:v>10.0656</x:v>
-      </x:c>
-      <x:c r="K2" s="61" t="str">
+      <x:c r="J2" s="67" t="n">
+        <x:v>10.0683</x:v>
+      </x:c>
+      <x:c r="K2" s="67" t="str">
         <x:v>AL16</x:v>
       </x:c>
-      <x:c r="L2" s="61" t="str">
+      <x:c r="L2" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M2" s="61" t="str">
+      <x:c r="M2" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N2" s="61" t="n">
+      <x:c r="N2" s="67" t="n">
         <x:v>47075</x:v>
       </x:c>
-      <x:c r="O2" s="61" t="n">
+      <x:c r="O2" s="67" t="n">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="P2" s="61" t="str">
+      <x:c r="P2" s="67" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="Q2" s="63" t="d">
+      <x:c r="Q2" s="69" t="d">
         <x:v>2019-08-14T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R2" s="63" t="d">
+      <x:c r="R2" s="69" t="d">
         <x:v>2039-02-20T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S2" s="61" t="str">
+      <x:c r="S2" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T2" s="61" t="str">
+      <x:c r="T2" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U2" s="61" t="n">
+      <x:c r="U2" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V2" s="61" t="str">
+      <x:c r="V2" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
-      <x:c r="B3" s="61" t="str">
+      <x:c r="B3" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C3" s="61" t="str">
+      <x:c r="C3" s="67" t="str">
         <x:v>S31612</x:v>
       </x:c>
-      <x:c r="D3" s="61" t="str">
+      <x:c r="D3" s="67" t="str">
         <x:v>Chan Ka</x:v>
       </x:c>
-      <x:c r="E3" s="61" t="str">
+      <x:c r="E3" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F3" s="61" t="str">
+      <x:c r="F3" s="67" t="str">
         <x:v>Assistant Manager 主管</x:v>
       </x:c>
-      <x:c r="G3" s="61" t="str">
+      <x:c r="G3" s="67" t="str">
         <x:v>OFFICER</x:v>
       </x:c>
-      <x:c r="H3" s="61" t="str">
+      <x:c r="H3" s="67" t="str">
         <x:v>OFFICER 主任</x:v>
       </x:c>
-      <x:c r="I3" s="63" t="d">
+      <x:c r="I3" s="69" t="d">
         <x:v>2016-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J3" s="61" t="n">
-        <x:v>4.2268</x:v>
-      </x:c>
-      <x:c r="K3" s="61" t="str">
+      <x:c r="J3" s="67" t="n">
+        <x:v>4.2295</x:v>
+      </x:c>
+      <x:c r="K3" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L3" s="61" t="str">
+      <x:c r="L3" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M3" s="61" t="str">
+      <x:c r="M3" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N3" s="61" t="n">
+      <x:c r="N3" s="67" t="n">
         <x:v>39554</x:v>
       </x:c>
-      <x:c r="O3" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P3" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q3" s="63" t="d">
+      <x:c r="O3" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P3" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q3" s="69" t="d">
         <x:v>2016-04-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R3" s="63" t="d">
+      <x:c r="R3" s="69" t="d">
         <x:v>2048-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S3" s="61" t="str">
+      <x:c r="S3" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T3" s="61" t="str">
+      <x:c r="T3" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U3" s="61" t="n">
+      <x:c r="U3" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V3" s="61" t="str">
+      <x:c r="V3" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
-      <x:c r="B4" s="61" t="str">
+      <x:c r="B4" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C4" s="61" t="str">
+      <x:c r="C4" s="67" t="str">
         <x:v>S31611</x:v>
       </x:c>
-      <x:c r="D4" s="61" t="str">
+      <x:c r="D4" s="67" t="str">
         <x:v>Chan Hang</x:v>
       </x:c>
-      <x:c r="E4" s="61" t="str">
+      <x:c r="E4" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F4" s="61" t="str">
+      <x:c r="F4" s="67" t="str">
         <x:v>Assistant Manager 主管</x:v>
       </x:c>
-      <x:c r="G4" s="61" t="str">
+      <x:c r="G4" s="67" t="str">
         <x:v>SUPERVISOR</x:v>
       </x:c>
-      <x:c r="H4" s="61" t="str">
+      <x:c r="H4" s="67" t="str">
         <x:v>主任</x:v>
       </x:c>
-      <x:c r="I4" s="63" t="d">
+      <x:c r="I4" s="69" t="d">
         <x:v>2016-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J4" s="61" t="n">
-        <x:v>4.2268</x:v>
-      </x:c>
-      <x:c r="K4" s="61" t="str">
+      <x:c r="J4" s="67" t="n">
+        <x:v>4.2295</x:v>
+      </x:c>
+      <x:c r="K4" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L4" s="61" t="str">
+      <x:c r="L4" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M4" s="61" t="str">
+      <x:c r="M4" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N4" s="61" t="n">
+      <x:c r="N4" s="67" t="n">
         <x:v>30020</x:v>
       </x:c>
-      <x:c r="O4" s="61" t="n">
+      <x:c r="O4" s="67" t="n">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="P4" s="61" t="str">
+      <x:c r="P4" s="67" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="Q4" s="63" t="d">
+      <x:c r="Q4" s="69" t="d">
         <x:v>2016-04-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R4" s="63" t="d">
+      <x:c r="R4" s="69" t="d">
         <x:v>2048-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S4" s="61" t="str">
+      <x:c r="S4" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T4" s="61" t="str">
+      <x:c r="T4" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U4" s="61" t="n">
+      <x:c r="U4" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V4" s="61" t="str">
+      <x:c r="V4" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
-      <x:c r="B5" s="61" t="str">
+      <x:c r="B5" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C5" s="61" t="str">
+      <x:c r="C5" s="67" t="str">
         <x:v>S30171</x:v>
       </x:c>
-      <x:c r="D5" s="61" t="str">
+      <x:c r="D5" s="67" t="str">
         <x:v>Chan Ka Man</x:v>
       </x:c>
-      <x:c r="E5" s="61" t="str">
+      <x:c r="E5" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F5" s="61" t="str">
+      <x:c r="F5" s="67" t="str">
         <x:v>Assistant Manager 主管</x:v>
       </x:c>
-      <x:c r="G5" s="61" t="str">
+      <x:c r="G5" s="67" t="str">
         <x:v>SW</x:v>
       </x:c>
-      <x:c r="H5" s="61" t="str">
+      <x:c r="H5" s="67" t="str">
         <x:v>SOCIAL WORKER 社會工作員</x:v>
       </x:c>
-      <x:c r="I5" s="63" t="d">
+      <x:c r="I5" s="69" t="d">
         <x:v>2011-10-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J5" s="61" t="n">
-        <x:v>8.4809</x:v>
-      </x:c>
-      <x:c r="K5" s="61" t="str">
+      <x:c r="J5" s="67" t="n">
+        <x:v>8.4836</x:v>
+      </x:c>
+      <x:c r="K5" s="67" t="str">
         <x:v>AL10</x:v>
       </x:c>
-      <x:c r="L5" s="61" t="str">
+      <x:c r="L5" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M5" s="61" t="str">
+      <x:c r="M5" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N5" s="61" t="n">
+      <x:c r="N5" s="67" t="n">
         <x:v>61170</x:v>
       </x:c>
-      <x:c r="O5" s="61" t="n">
+      <x:c r="O5" s="67" t="n">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="P5" s="61" t="str">
+      <x:c r="P5" s="67" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="Q5" s="63" t="d">
+      <x:c r="Q5" s="69" t="d">
         <x:v>2018-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R5" s="63" t="d">
+      <x:c r="R5" s="69" t="d">
         <x:v>2020-08-31T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S5" s="61" t="str">
+      <x:c r="S5" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T5" s="61" t="str">
+      <x:c r="T5" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U5" s="61" t="n">
+      <x:c r="U5" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V5" s="61" t="str">
+      <x:c r="V5" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
-      <x:c r="B6" s="61" t="str">
+      <x:c r="B6" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C6" s="61" t="str">
+      <x:c r="C6" s="67" t="str">
         <x:v>S31655</x:v>
       </x:c>
-      <x:c r="D6" s="61" t="str">
+      <x:c r="D6" s="67" t="str">
         <x:v>Wong Chung</x:v>
       </x:c>
-      <x:c r="E6" s="61" t="str">
+      <x:c r="E6" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F6" s="61" t="str">
+      <x:c r="F6" s="67" t="str">
         <x:v>Executive Level 管理層</x:v>
       </x:c>
-      <x:c r="G6" s="61" t="str">
+      <x:c r="G6" s="67" t="str">
         <x:v>SSW</x:v>
       </x:c>
-      <x:c r="H6" s="61" t="str">
+      <x:c r="H6" s="67" t="str">
         <x:v>Senior Social  资深社工</x:v>
       </x:c>
-      <x:c r="I6" s="63" t="d">
+      <x:c r="I6" s="69" t="d">
         <x:v>2012-05-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J6" s="61" t="n">
-        <x:v>7.8962</x:v>
-      </x:c>
-      <x:c r="K6" s="61" t="str">
+      <x:c r="J6" s="67" t="n">
+        <x:v>7.8989</x:v>
+      </x:c>
+      <x:c r="K6" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L6" s="61" t="str">
+      <x:c r="L6" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M6" s="61" t="str">
+      <x:c r="M6" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N6" s="61" t="n">
+      <x:c r="N6" s="67" t="n">
         <x:v>26000</x:v>
       </x:c>
-      <x:c r="O6" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P6" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q6" s="63" t="d">
+      <x:c r="O6" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P6" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q6" s="69" t="d">
         <x:v>2012-05-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R6" s="63" t="d">
+      <x:c r="R6" s="69" t="d">
         <x:v>2053-02-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S6" s="61" t="str">
+      <x:c r="S6" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T6" s="61" t="str">
+      <x:c r="T6" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U6" s="61" t="n">
+      <x:c r="U6" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V6" s="61" t="str">
+      <x:c r="V6" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
-      <x:c r="B7" s="61" t="str">
+      <x:c r="B7" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C7" s="61" t="str">
+      <x:c r="C7" s="67" t="str">
         <x:v>S31629</x:v>
       </x:c>
-      <x:c r="D7" s="61" t="str">
+      <x:c r="D7" s="67" t="str">
         <x:v>Lee Siu</x:v>
       </x:c>
-      <x:c r="E7" s="61" t="str">
+      <x:c r="E7" s="67" t="str">
         <x:v>Unit C</x:v>
       </x:c>
-      <x:c r="F7" s="61" t="str">
+      <x:c r="F7" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G7" s="61" t="str">
+      <x:c r="G7" s="67" t="str">
         <x:v>CLEANER</x:v>
       </x:c>
-      <x:c r="H7" s="61" t="str">
+      <x:c r="H7" s="67" t="str">
         <x:v>CLEANER 清潔員</x:v>
       </x:c>
-      <x:c r="I7" s="63" t="d">
+      <x:c r="I7" s="69" t="d">
         <x:v>2016-07-04T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J7" s="61" t="n">
-        <x:v>3.724</x:v>
-      </x:c>
-      <x:c r="K7" s="61" t="str">
+      <x:c r="J7" s="67" t="n">
+        <x:v>3.7268</x:v>
+      </x:c>
+      <x:c r="K7" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L7" s="61" t="str">
+      <x:c r="L7" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M7" s="61" t="str">
+      <x:c r="M7" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N7" s="61" t="n">
+      <x:c r="N7" s="67" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="O7" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P7" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q7" s="63" t="d">
+      <x:c r="O7" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P7" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q7" s="69" t="d">
         <x:v>2016-07-04T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R7" s="63" t="d">
+      <x:c r="R7" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S7" s="61" t="str">
+      <x:c r="S7" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T7" s="61" t="str">
+      <x:c r="T7" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U7" s="61" t="n">
+      <x:c r="U7" s="67" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="V7" s="61" t="str">
+      <x:c r="V7" s="67" t="str">
         <x:v>TST</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
-      <x:c r="B8" s="61" t="str">
+      <x:c r="B8" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C8" s="61" t="str">
+      <x:c r="C8" s="67" t="str">
         <x:v>S31641</x:v>
       </x:c>
-      <x:c r="D8" s="61" t="str">
+      <x:c r="D8" s="67" t="str">
         <x:v>Wong Li Chun</x:v>
       </x:c>
-      <x:c r="E8" s="61" t="str">
+      <x:c r="E8" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F8" s="61" t="str">
+      <x:c r="F8" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G8" s="61" t="str">
+      <x:c r="G8" s="67" t="str">
         <x:v>CLEANER</x:v>
       </x:c>
-      <x:c r="H8" s="61" t="str">
+      <x:c r="H8" s="67" t="str">
         <x:v>CLEANER 清潔員</x:v>
       </x:c>
-      <x:c r="I8" s="63" t="d">
+      <x:c r="I8" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J8" s="61" t="n">
-        <x:v>2.224</x:v>
-      </x:c>
-      <x:c r="K8" s="61" t="str">
+      <x:c r="J8" s="67" t="n">
+        <x:v>2.2268</x:v>
+      </x:c>
+      <x:c r="K8" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L8" s="61" t="str">
+      <x:c r="L8" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M8" s="61" t="str">
+      <x:c r="M8" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N8" s="61" t="n">
+      <x:c r="N8" s="67" t="n">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="O8" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P8" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q8" s="63" t="d">
+      <x:c r="O8" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P8" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q8" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R8" s="63" t="d">
+      <x:c r="R8" s="69" t="d">
         <x:v>2053-08-08T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S8" s="61" t="str">
+      <x:c r="S8" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T8" s="61" t="str">
+      <x:c r="T8" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U8" s="61" t="n">
+      <x:c r="U8" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V8" s="61" t="str">
+      <x:c r="V8" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
-      <x:c r="B9" s="61" t="str">
+      <x:c r="B9" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C9" s="61" t="str">
+      <x:c r="C9" s="67" t="str">
         <x:v>S31646</x:v>
       </x:c>
-      <x:c r="D9" s="61" t="str">
+      <x:c r="D9" s="67" t="str">
         <x:v>Li Yim Fong2</x:v>
       </x:c>
-      <x:c r="E9" s="61" t="str">
+      <x:c r="E9" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F9" s="61" t="str">
+      <x:c r="F9" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G9" s="61" t="str">
+      <x:c r="G9" s="67" t="str">
         <x:v>CLEANER</x:v>
       </x:c>
-      <x:c r="H9" s="61" t="str">
+      <x:c r="H9" s="67" t="str">
         <x:v>CLEANER 清潔員</x:v>
       </x:c>
-      <x:c r="I9" s="63" t="d">
+      <x:c r="I9" s="69" t="d">
         <x:v>2016-11-28T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J9" s="61" t="n">
-        <x:v>3.3224</x:v>
-      </x:c>
-      <x:c r="K9" s="61" t="str">
+      <x:c r="J9" s="67" t="n">
+        <x:v>3.3251</x:v>
+      </x:c>
+      <x:c r="K9" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L9" s="61" t="str">
+      <x:c r="L9" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M9" s="61" t="str">
+      <x:c r="M9" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N9" s="61" t="n">
+      <x:c r="N9" s="67" t="n">
         <x:v>74</x:v>
       </x:c>
-      <x:c r="O9" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P9" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q9" s="63" t="d">
+      <x:c r="O9" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P9" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q9" s="69" t="d">
         <x:v>2016-11-28T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R9" s="63" t="d">
+      <x:c r="R9" s="69" t="d">
         <x:v>2053-04-07T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S9" s="61" t="str">
+      <x:c r="S9" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T9" s="61" t="str">
+      <x:c r="T9" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U9" s="61" t="n">
+      <x:c r="U9" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V9" s="61" t="str">
+      <x:c r="V9" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
-      <x:c r="B10" s="61" t="str">
+      <x:c r="B10" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C10" s="61" t="str">
+      <x:c r="C10" s="67" t="str">
         <x:v>S31648</x:v>
       </x:c>
-      <x:c r="D10" s="61" t="str">
+      <x:c r="D10" s="67" t="str">
         <x:v>Lau Mei Lan</x:v>
       </x:c>
-      <x:c r="E10" s="61" t="str">
+      <x:c r="E10" s="67" t="str">
         <x:v>Unit C</x:v>
       </x:c>
-      <x:c r="F10" s="61" t="str">
+      <x:c r="F10" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G10" s="61" t="str">
+      <x:c r="G10" s="67" t="str">
         <x:v>CLEANER</x:v>
       </x:c>
-      <x:c r="H10" s="61" t="str">
+      <x:c r="H10" s="67" t="str">
         <x:v>CLEANER 清潔員</x:v>
       </x:c>
-      <x:c r="I10" s="63" t="d">
+      <x:c r="I10" s="69" t="d">
         <x:v>2017-02-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J10" s="61" t="n">
-        <x:v>3.1421</x:v>
-      </x:c>
-      <x:c r="K10" s="61" t="str">
+      <x:c r="J10" s="67" t="n">
+        <x:v>3.1448</x:v>
+      </x:c>
+      <x:c r="K10" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L10" s="61" t="str">
+      <x:c r="L10" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M10" s="61" t="str">
+      <x:c r="M10" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N10" s="61" t="n">
+      <x:c r="N10" s="67" t="n">
         <x:v>6000</x:v>
       </x:c>
-      <x:c r="O10" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P10" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q10" s="63" t="d">
+      <x:c r="O10" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P10" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q10" s="69" t="d">
         <x:v>2017-02-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R10" s="63" t="d">
+      <x:c r="R10" s="69" t="d">
         <x:v>2053-03-22T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S10" s="61" t="str">
+      <x:c r="S10" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T10" s="61" t="str">
+      <x:c r="T10" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U10" s="61" t="n">
+      <x:c r="U10" s="67" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="V10" s="61" t="str">
+      <x:c r="V10" s="67" t="str">
         <x:v>TST</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
-      <x:c r="B11" s="61" t="str">
+      <x:c r="B11" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C11" s="61" t="str">
+      <x:c r="C11" s="67" t="str">
         <x:v>AA100003</x:v>
       </x:c>
-      <x:c r="D11" s="61" t="str">
+      <x:c r="D11" s="67" t="str">
         <x:v>DWS 190808</x:v>
       </x:c>
-      <x:c r="E11" s="61" t="str">
+      <x:c r="E11" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F11" s="61" t="str">
+      <x:c r="F11" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G11" s="61" t="str">
+      <x:c r="G11" s="67" t="str">
         <x:v>CLERK</x:v>
       </x:c>
-      <x:c r="H11" s="61" t="str">
+      <x:c r="H11" s="67" t="str">
         <x:v>CLERK 文員</x:v>
       </x:c>
-      <x:c r="I11" s="63" t="d">
+      <x:c r="I11" s="69" t="d">
         <x:v>2019-05-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J11" s="61" t="n">
-        <x:v>0.8989</x:v>
-      </x:c>
-      <x:c r="K11" s="61" t="str">
+      <x:c r="J11" s="67" t="n">
+        <x:v>0.9016</x:v>
+      </x:c>
+      <x:c r="K11" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L11" s="61" t="str">
+      <x:c r="L11" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M11" s="61" t="str">
+      <x:c r="M11" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N11" s="61" t="n">
+      <x:c r="N11" s="67" t="n">
         <x:v>7000</x:v>
       </x:c>
-      <x:c r="O11" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P11" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q11" s="63" t="d">
+      <x:c r="O11" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P11" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q11" s="69" t="d">
         <x:v>2019-05-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R11" s="63" t="d">
+      <x:c r="R11" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S11" s="61" t="str">
+      <x:c r="S11" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T11" s="61" t="str">
+      <x:c r="T11" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U11" s="61" t="n">
+      <x:c r="U11" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V11" s="61" t="str">
+      <x:c r="V11" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
-      <x:c r="B12" s="61" t="str">
+      <x:c r="B12" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C12" s="61" t="str">
+      <x:c r="C12" s="67" t="str">
         <x:v>AA100821</x:v>
       </x:c>
-      <x:c r="D12" s="61" t="str">
+      <x:c r="D12" s="67" t="str">
         <x:v>Sheung Foon Lok</x:v>
       </x:c>
-      <x:c r="E12" s="61" t="str">
+      <x:c r="E12" s="67" t="str">
         <x:v>CLP</x:v>
       </x:c>
-      <x:c r="F12" s="61" t="str">
+      <x:c r="F12" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G12" s="61" t="str">
+      <x:c r="G12" s="67" t="str">
         <x:v>CLERK</x:v>
       </x:c>
-      <x:c r="H12" s="61" t="str">
+      <x:c r="H12" s="67" t="str">
         <x:v>CLERK 文員</x:v>
       </x:c>
-      <x:c r="I12" s="63" t="d">
+      <x:c r="I12" s="69" t="d">
         <x:v>2019-10-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J12" s="61" t="n">
-        <x:v>0.4781</x:v>
-      </x:c>
-      <x:c r="K12" s="61" t="str">
+      <x:c r="J12" s="67" t="n">
+        <x:v>0.4809</x:v>
+      </x:c>
+      <x:c r="K12" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L12" s="61" t="str">
+      <x:c r="L12" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M12" s="61" t="str">
+      <x:c r="M12" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N12" s="61" t="n">
+      <x:c r="N12" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O12" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P12" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q12" s="63" t="d">
+      <x:c r="O12" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P12" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q12" s="69" t="d">
         <x:v>2019-10-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R12" s="63" t="d">
+      <x:c r="R12" s="69" t="d">
         <x:v>2022-10-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S12" s="61" t="str">
+      <x:c r="S12" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T12" s="61" t="str">
+      <x:c r="T12" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U12" s="61" t="n">
+      <x:c r="U12" s="67" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="V12" s="61" t="str">
+      <x:c r="V12" s="67" t="str">
         <x:v>TST</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
-      <x:c r="B13" s="61" t="str">
+      <x:c r="B13" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C13" s="61" t="str">
+      <x:c r="C13" s="67" t="str">
         <x:v>AA100824</x:v>
       </x:c>
-      <x:c r="D13" s="61" t="str">
+      <x:c r="D13" s="67" t="str">
         <x:v>linson liang</x:v>
       </x:c>
-      <x:c r="E13" s="61" t="str">
+      <x:c r="E13" s="67" t="str">
         <x:v>CLP</x:v>
       </x:c>
-      <x:c r="F13" s="61" t="str">
+      <x:c r="F13" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G13" s="61" t="str">
+      <x:c r="G13" s="67" t="str">
         <x:v>CLERK</x:v>
       </x:c>
-      <x:c r="H13" s="61" t="str">
+      <x:c r="H13" s="67" t="str">
         <x:v>CLERK 文員</x:v>
       </x:c>
-      <x:c r="I13" s="63" t="d">
+      <x:c r="I13" s="69" t="d">
         <x:v>2020-03-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J13" s="61" t="n">
-        <x:v>0.041</x:v>
-      </x:c>
-      <x:c r="K13" s="61" t="str">
+      <x:c r="J13" s="67" t="n">
+        <x:v>0.0437</x:v>
+      </x:c>
+      <x:c r="K13" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L13" s="61" t="str">
+      <x:c r="L13" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M13" s="61" t="str">
+      <x:c r="M13" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N13" s="61" t="n">
+      <x:c r="N13" s="67" t="n">
         <x:v>35000</x:v>
       </x:c>
-      <x:c r="O13" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P13" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q13" s="63" t="d">
+      <x:c r="O13" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P13" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q13" s="69" t="d">
         <x:v>2020-03-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R13" s="63" t="d">
+      <x:c r="R13" s="69" t="d">
         <x:v>2053-08-08T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S13" s="61" t="str">
+      <x:c r="S13" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T13" s="61" t="str">
+      <x:c r="T13" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U13" s="61" t="n">
+      <x:c r="U13" s="67" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="V13" s="61" t="str">
+      <x:c r="V13" s="67" t="str">
         <x:v>Account Department</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
-      <x:c r="B14" s="61" t="str">
+      <x:c r="B14" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C14" s="61" t="str">
+      <x:c r="C14" s="67" t="str">
         <x:v>S31636</x:v>
       </x:c>
-      <x:c r="D14" s="61" t="str">
+      <x:c r="D14" s="67" t="str">
         <x:v>Chan Man Hung</x:v>
       </x:c>
-      <x:c r="E14" s="61" t="str">
+      <x:c r="E14" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F14" s="61" t="str">
+      <x:c r="F14" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G14" s="61" t="str">
+      <x:c r="G14" s="67" t="str">
         <x:v>CLERK</x:v>
       </x:c>
-      <x:c r="H14" s="61" t="str">
+      <x:c r="H14" s="67" t="str">
         <x:v>CLERK 文員</x:v>
       </x:c>
-      <x:c r="I14" s="63" t="d">
+      <x:c r="I14" s="69" t="d">
         <x:v>2017-03-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J14" s="61" t="n">
-        <x:v>3.0656</x:v>
-      </x:c>
-      <x:c r="K14" s="61" t="str">
+      <x:c r="J14" s="67" t="n">
+        <x:v>3.0683</x:v>
+      </x:c>
+      <x:c r="K14" s="67" t="str">
         <x:v>AL10</x:v>
       </x:c>
-      <x:c r="L14" s="61" t="str">
+      <x:c r="L14" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M14" s="61" t="str">
+      <x:c r="M14" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N14" s="61" t="n">
+      <x:c r="N14" s="67" t="n">
         <x:v>70</x:v>
       </x:c>
-      <x:c r="O14" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P14" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q14" s="63" t="d">
+      <x:c r="O14" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P14" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q14" s="69" t="d">
         <x:v>2018-09-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R14" s="63" t="d">
+      <x:c r="R14" s="69" t="d">
         <x:v>2037-02-03T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S14" s="61" t="str">
+      <x:c r="S14" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T14" s="61" t="str">
+      <x:c r="T14" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U14" s="61" t="n">
+      <x:c r="U14" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V14" s="61" t="str">
+      <x:c r="V14" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
-      <x:c r="B15" s="61" t="str">
+      <x:c r="B15" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C15" s="61" t="str">
+      <x:c r="C15" s="67" t="str">
         <x:v>S31642</x:v>
       </x:c>
-      <x:c r="D15" s="61" t="str">
+      <x:c r="D15" s="67" t="str">
         <x:v>Chan Siu Fong</x:v>
       </x:c>
-      <x:c r="E15" s="61" t="str">
+      <x:c r="E15" s="67" t="str">
         <x:v>Unit C</x:v>
       </x:c>
-      <x:c r="F15" s="61" t="str">
+      <x:c r="F15" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G15" s="61" t="str">
+      <x:c r="G15" s="67" t="str">
         <x:v>CLERK</x:v>
       </x:c>
-      <x:c r="H15" s="61" t="str">
+      <x:c r="H15" s="67" t="str">
         <x:v>CLERK 文員</x:v>
       </x:c>
-      <x:c r="I15" s="63" t="d">
+      <x:c r="I15" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J15" s="61" t="n">
-        <x:v>2.224</x:v>
-      </x:c>
-      <x:c r="K15" s="61" t="str">
+      <x:c r="J15" s="67" t="n">
+        <x:v>2.2268</x:v>
+      </x:c>
+      <x:c r="K15" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L15" s="61" t="str">
+      <x:c r="L15" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M15" s="61" t="str">
+      <x:c r="M15" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N15" s="61" t="n">
+      <x:c r="N15" s="67" t="n">
         <x:v>9000</x:v>
       </x:c>
-      <x:c r="O15" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P15" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q15" s="63" t="d">
+      <x:c r="O15" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P15" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q15" s="69" t="d">
         <x:v>2019-08-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R15" s="63" t="d">
+      <x:c r="R15" s="69" t="d">
         <x:v>2040-02-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S15" s="61" t="str">
+      <x:c r="S15" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T15" s="61" t="str">
+      <x:c r="T15" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U15" s="61" t="n">
+      <x:c r="U15" s="67" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="V15" s="61" t="str">
+      <x:c r="V15" s="67" t="str">
         <x:v>TST</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
-      <x:c r="B16" s="61" t="str">
+      <x:c r="B16" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C16" s="61" t="str">
+      <x:c r="C16" s="67" t="str">
         <x:v>AA100818</x:v>
       </x:c>
-      <x:c r="D16" s="61" t="str">
+      <x:c r="D16" s="67" t="str">
         <x:v>Chan Tai man 10</x:v>
       </x:c>
-      <x:c r="E16" s="61" t="str">
+      <x:c r="E16" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F16" s="61" t="str">
+      <x:c r="F16" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G16" s="61" t="str">
+      <x:c r="G16" s="67" t="str">
         <x:v>CWIII</x:v>
       </x:c>
-      <x:c r="H16" s="61" t="str">
+      <x:c r="H16" s="67" t="str">
         <x:v>CARE WORKER 護理員</x:v>
       </x:c>
-      <x:c r="I16" s="63" t="d">
+      <x:c r="I16" s="69" t="d">
         <x:v>2019-10-11T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J16" s="61" t="n">
-        <x:v>0.4536</x:v>
-      </x:c>
-      <x:c r="K16" s="61" t="str">
+      <x:c r="J16" s="67" t="n">
+        <x:v>0.4563</x:v>
+      </x:c>
+      <x:c r="K16" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L16" s="61" t="str">
+      <x:c r="L16" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M16" s="61" t="str">
+      <x:c r="M16" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N16" s="61" t="n">
+      <x:c r="N16" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O16" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P16" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q16" s="63" t="d">
+      <x:c r="O16" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P16" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q16" s="69" t="d">
         <x:v>2019-10-11T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R16" s="63" t="d">
+      <x:c r="R16" s="69" t="d">
         <x:v>2020-10-11T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S16" s="61" t="str">
+      <x:c r="S16" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T16" s="61" t="str">
+      <x:c r="T16" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U16" s="61" t="n">
+      <x:c r="U16" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V16" s="61" t="str">
+      <x:c r="V16" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
-      <x:c r="B17" s="61" t="str">
+      <x:c r="B17" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C17" s="61" t="str">
+      <x:c r="C17" s="67" t="str">
         <x:v>AA100820</x:v>
       </x:c>
-      <x:c r="D17" s="61" t="str">
+      <x:c r="D17" s="67" t="str">
         <x:v>DWS 191108</x:v>
       </x:c>
-      <x:c r="E17" s="61" t="str">
+      <x:c r="E17" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F17" s="61" t="str">
+      <x:c r="F17" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G17" s="61" t="str">
+      <x:c r="G17" s="67" t="str">
         <x:v>CWIII</x:v>
       </x:c>
-      <x:c r="H17" s="61" t="str">
+      <x:c r="H17" s="67" t="str">
         <x:v>CARE WORKER 護理員</x:v>
       </x:c>
-      <x:c r="I17" s="63" t="d">
+      <x:c r="I17" s="69" t="d">
         <x:v>2019-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J17" s="61" t="n">
-        <x:v>0.3962</x:v>
-      </x:c>
-      <x:c r="K17" s="61" t="str">
+      <x:c r="J17" s="67" t="n">
+        <x:v>0.3989</x:v>
+      </x:c>
+      <x:c r="K17" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L17" s="61" t="str">
+      <x:c r="L17" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M17" s="61" t="str">
+      <x:c r="M17" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N17" s="61" t="n">
+      <x:c r="N17" s="67" t="n">
         <x:v>17080</x:v>
       </x:c>
-      <x:c r="O17" s="61" t="n">
+      <x:c r="O17" s="67" t="n">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="P17" s="61" t="str">
+      <x:c r="P17" s="67" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="Q17" s="63" t="d">
+      <x:c r="Q17" s="69" t="d">
         <x:v>2019-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R17" s="63" t="d">
+      <x:c r="R17" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S17" s="61" t="str">
+      <x:c r="S17" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T17" s="61" t="str">
+      <x:c r="T17" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U17" s="61" t="n">
+      <x:c r="U17" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V17" s="61" t="str">
+      <x:c r="V17" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
-      <x:c r="B18" s="61" t="str">
+      <x:c r="B18" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C18" s="61" t="str">
+      <x:c r="C18" s="67" t="str">
         <x:v>AA100002</x:v>
       </x:c>
-      <x:c r="D18" s="61" t="str">
+      <x:c r="D18" s="67" t="str">
         <x:v>Test One</x:v>
       </x:c>
-      <x:c r="E18" s="61" t="str">
+      <x:c r="E18" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F18" s="61" t="str">
+      <x:c r="F18" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G18" s="61" t="str">
+      <x:c r="G18" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H18" s="61" t="str">
+      <x:c r="H18" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I18" s="63" t="d">
+      <x:c r="I18" s="69" t="d">
         <x:v>2019-07-15T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J18" s="61" t="n">
-        <x:v>0.694</x:v>
-      </x:c>
-      <x:c r="K18" s="61" t="str">
+      <x:c r="J18" s="67" t="n">
+        <x:v>0.6967</x:v>
+      </x:c>
+      <x:c r="K18" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L18" s="61" t="str">
+      <x:c r="L18" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M18" s="61" t="str">
+      <x:c r="M18" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N18" s="61" t="n">
+      <x:c r="N18" s="67" t="n">
         <x:v>12000</x:v>
       </x:c>
-      <x:c r="O18" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P18" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q18" s="63" t="d">
+      <x:c r="O18" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P18" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q18" s="69" t="d">
         <x:v>2019-07-15T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R18" s="63" t="d">
+      <x:c r="R18" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S18" s="61" t="str">
+      <x:c r="S18" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T18" s="61" t="str">
+      <x:c r="T18" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U18" s="61" t="n">
+      <x:c r="U18" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V18" s="61" t="str">
+      <x:c r="V18" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
-      <x:c r="B19" s="61" t="str">
+      <x:c r="B19" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C19" s="61" t="str">
+      <x:c r="C19" s="67" t="str">
         <x:v>AA100819</x:v>
       </x:c>
-      <x:c r="D19" s="61" t="str">
+      <x:c r="D19" s="67" t="str">
         <x:v>demo 191028</x:v>
       </x:c>
-      <x:c r="E19" s="61" t="str">
+      <x:c r="E19" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F19" s="61" t="str">
+      <x:c r="F19" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G19" s="61" t="str">
+      <x:c r="G19" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H19" s="61" t="str">
+      <x:c r="H19" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I19" s="63" t="d">
+      <x:c r="I19" s="69" t="d">
         <x:v>2019-10-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J19" s="61" t="n">
-        <x:v>0.4809</x:v>
-      </x:c>
-      <x:c r="K19" s="61" t="str">
+      <x:c r="J19" s="67" t="n">
+        <x:v>0.4836</x:v>
+      </x:c>
+      <x:c r="K19" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L19" s="61" t="str">
+      <x:c r="L19" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M19" s="61" t="str">
+      <x:c r="M19" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N19" s="61" t="n">
+      <x:c r="N19" s="67" t="n">
         <x:v>15730</x:v>
       </x:c>
-      <x:c r="O19" s="61" t="n">
+      <x:c r="O19" s="67" t="n">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="P19" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q19" s="63" t="d">
+      <x:c r="P19" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q19" s="69" t="d">
         <x:v>2019-10-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R19" s="63" t="d">
+      <x:c r="R19" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S19" s="61" t="str">
+      <x:c r="S19" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T19" s="61" t="str">
+      <x:c r="T19" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U19" s="61" t="n">
+      <x:c r="U19" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V19" s="61" t="str">
+      <x:c r="V19" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
-      <x:c r="B20" s="61" t="str">
+      <x:c r="B20" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C20" s="61" t="str">
+      <x:c r="C20" s="67" t="str">
         <x:v>S31609</x:v>
       </x:c>
-      <x:c r="D20" s="61" t="str">
+      <x:c r="D20" s="67" t="str">
         <x:v>Chan Fai</x:v>
       </x:c>
-      <x:c r="E20" s="61" t="str">
+      <x:c r="E20" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F20" s="61" t="str">
+      <x:c r="F20" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G20" s="61" t="str">
+      <x:c r="G20" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H20" s="61" t="str">
+      <x:c r="H20" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I20" s="63" t="d">
+      <x:c r="I20" s="69" t="d">
         <x:v>2016-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J20" s="61" t="n">
-        <x:v>4.2268</x:v>
-      </x:c>
-      <x:c r="K20" s="61" t="str">
+      <x:c r="J20" s="67" t="n">
+        <x:v>4.2295</x:v>
+      </x:c>
+      <x:c r="K20" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L20" s="61" t="str">
+      <x:c r="L20" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M20" s="61" t="str">
+      <x:c r="M20" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N20" s="61" t="n">
+      <x:c r="N20" s="67" t="n">
         <x:v>22005</x:v>
       </x:c>
-      <x:c r="O20" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P20" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q20" s="63" t="d">
+      <x:c r="O20" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P20" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q20" s="69" t="d">
         <x:v>2019-08-14T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R20" s="63" t="d">
+      <x:c r="R20" s="69" t="d">
         <x:v>2034-05-05T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S20" s="61" t="str">
+      <x:c r="S20" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T20" s="61" t="str">
+      <x:c r="T20" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U20" s="61" t="n">
+      <x:c r="U20" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V20" s="61" t="str">
+      <x:c r="V20" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="21">
-      <x:c r="B21" s="61" t="str">
+      <x:c r="B21" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C21" s="61" t="str">
+      <x:c r="C21" s="67" t="str">
         <x:v>S31610</x:v>
       </x:c>
-      <x:c r="D21" s="61" t="str">
+      <x:c r="D21" s="67" t="str">
         <x:v>Chan Shun</x:v>
       </x:c>
-      <x:c r="E21" s="61" t="str">
+      <x:c r="E21" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F21" s="61" t="str">
+      <x:c r="F21" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G21" s="61" t="str">
+      <x:c r="G21" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H21" s="61" t="str">
+      <x:c r="H21" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I21" s="63" t="d">
+      <x:c r="I21" s="69" t="d">
         <x:v>2016-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J21" s="61" t="n">
-        <x:v>4.2268</x:v>
-      </x:c>
-      <x:c r="K21" s="61" t="str">
+      <x:c r="J21" s="67" t="n">
+        <x:v>4.2295</x:v>
+      </x:c>
+      <x:c r="K21" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L21" s="61" t="str">
+      <x:c r="L21" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M21" s="61" t="str">
+      <x:c r="M21" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N21" s="61" t="n">
+      <x:c r="N21" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O21" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P21" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q21" s="63" t="d">
+      <x:c r="O21" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P21" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q21" s="69" t="d">
         <x:v>2018-12-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R21" s="63" t="d">
+      <x:c r="R21" s="69" t="d">
         <x:v>2046-06-06T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S21" s="61" t="str">
+      <x:c r="S21" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T21" s="61" t="str">
+      <x:c r="T21" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U21" s="61" t="n">
+      <x:c r="U21" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V21" s="61" t="str">
+      <x:c r="V21" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="22">
-      <x:c r="B22" s="61" t="str">
+      <x:c r="B22" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C22" s="61" t="str">
+      <x:c r="C22" s="67" t="str">
         <x:v>S31643</x:v>
       </x:c>
-      <x:c r="D22" s="61" t="str">
+      <x:c r="D22" s="67" t="str">
         <x:v>Chan Li Chun</x:v>
       </x:c>
-      <x:c r="E22" s="61" t="str">
+      <x:c r="E22" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F22" s="61" t="str">
+      <x:c r="F22" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G22" s="61" t="str">
+      <x:c r="G22" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H22" s="61" t="str">
+      <x:c r="H22" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I22" s="63" t="d">
+      <x:c r="I22" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J22" s="61" t="n">
-        <x:v>2.224</x:v>
-      </x:c>
-      <x:c r="K22" s="61" t="str">
+      <x:c r="J22" s="67" t="n">
+        <x:v>2.2268</x:v>
+      </x:c>
+      <x:c r="K22" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L22" s="61" t="str">
+      <x:c r="L22" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M22" s="61" t="str">
+      <x:c r="M22" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N22" s="61" t="n">
+      <x:c r="N22" s="67" t="n">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="O22" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P22" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q22" s="63" t="d">
+      <x:c r="O22" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P22" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q22" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R22" s="63" t="d">
+      <x:c r="R22" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S22" s="61" t="str">
+      <x:c r="S22" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T22" s="61" t="str">
+      <x:c r="T22" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U22" s="61" t="n">
+      <x:c r="U22" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V22" s="61" t="str">
+      <x:c r="V22" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="23">
-      <x:c r="B23" s="61" t="str">
+      <x:c r="B23" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C23" s="61" t="str">
+      <x:c r="C23" s="67" t="str">
         <x:v>S31644</x:v>
       </x:c>
-      <x:c r="D23" s="61" t="str">
+      <x:c r="D23" s="67" t="str">
         <x:v>Cheung Li Chun</x:v>
       </x:c>
-      <x:c r="E23" s="61" t="str">
+      <x:c r="E23" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F23" s="61" t="str">
+      <x:c r="F23" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G23" s="61" t="str">
+      <x:c r="G23" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H23" s="61" t="str">
+      <x:c r="H23" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I23" s="63" t="d">
+      <x:c r="I23" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J23" s="61" t="n">
-        <x:v>2.224</x:v>
-      </x:c>
-      <x:c r="K23" s="61" t="str">
+      <x:c r="J23" s="67" t="n">
+        <x:v>2.2268</x:v>
+      </x:c>
+      <x:c r="K23" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L23" s="61" t="str">
+      <x:c r="L23" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M23" s="61" t="str">
+      <x:c r="M23" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N23" s="61" t="n">
+      <x:c r="N23" s="67" t="n">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="O23" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P23" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q23" s="63" t="d">
+      <x:c r="O23" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P23" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q23" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R23" s="63" t="d">
+      <x:c r="R23" s="69" t="d">
         <x:v>2041-03-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S23" s="61" t="str">
+      <x:c r="S23" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T23" s="61" t="str">
+      <x:c r="T23" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U23" s="61" t="n">
+      <x:c r="U23" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V23" s="61" t="str">
+      <x:c r="V23" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="24">
-      <x:c r="B24" s="61" t="str">
+      <x:c r="B24" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C24" s="61" t="str">
+      <x:c r="C24" s="67" t="str">
         <x:v>S31645</x:v>
       </x:c>
-      <x:c r="D24" s="61" t="str">
+      <x:c r="D24" s="67" t="str">
         <x:v>Chan Siu Li</x:v>
       </x:c>
-      <x:c r="E24" s="61" t="str">
+      <x:c r="E24" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F24" s="61" t="str">
+      <x:c r="F24" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G24" s="61" t="str">
+      <x:c r="G24" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H24" s="61" t="str">
+      <x:c r="H24" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I24" s="63" t="d">
+      <x:c r="I24" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J24" s="61" t="n">
-        <x:v>2.224</x:v>
-      </x:c>
-      <x:c r="K24" s="61" t="str">
+      <x:c r="J24" s="67" t="n">
+        <x:v>2.2268</x:v>
+      </x:c>
+      <x:c r="K24" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L24" s="61" t="str">
+      <x:c r="L24" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M24" s="61" t="str">
+      <x:c r="M24" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N24" s="61" t="n">
+      <x:c r="N24" s="67" t="n">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="O24" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P24" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q24" s="63" t="d">
+      <x:c r="O24" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P24" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q24" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R24" s="63" t="d">
+      <x:c r="R24" s="69" t="d">
         <x:v>2050-12-15T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S24" s="61" t="str">
+      <x:c r="S24" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T24" s="61" t="str">
+      <x:c r="T24" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U24" s="61" t="n">
+      <x:c r="U24" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V24" s="61" t="str">
+      <x:c r="V24" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="25">
-      <x:c r="B25" s="61" t="str">
+      <x:c r="B25" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C25" s="61" t="str">
+      <x:c r="C25" s="67" t="str">
         <x:v>S31647</x:v>
       </x:c>
-      <x:c r="D25" s="61" t="str">
+      <x:c r="D25" s="67" t="str">
         <x:v>Chan guan guan</x:v>
       </x:c>
-      <x:c r="E25" s="61" t="str">
+      <x:c r="E25" s="67" t="str">
         <x:v>Unit B</x:v>
       </x:c>
-      <x:c r="F25" s="61" t="str">
+      <x:c r="F25" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G25" s="61" t="str">
+      <x:c r="G25" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H25" s="61" t="str">
+      <x:c r="H25" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I25" s="63" t="d">
+      <x:c r="I25" s="69" t="d">
         <x:v>2015-11-15T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J25" s="61" t="n">
-        <x:v>4.3579</x:v>
-      </x:c>
-      <x:c r="K25" s="61" t="str">
+      <x:c r="J25" s="67" t="n">
+        <x:v>4.3607</x:v>
+      </x:c>
+      <x:c r="K25" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L25" s="61" t="str">
+      <x:c r="L25" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M25" s="61" t="str">
+      <x:c r="M25" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N25" s="61" t="n">
+      <x:c r="N25" s="67" t="n">
         <x:v>15000</x:v>
       </x:c>
-      <x:c r="O25" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P25" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q25" s="63" t="d">
+      <x:c r="O25" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P25" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q25" s="69" t="d">
         <x:v>2019-09-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R25" s="63" t="d">
+      <x:c r="R25" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S25" s="61" t="str">
+      <x:c r="S25" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T25" s="61" t="str">
+      <x:c r="T25" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U25" s="61" t="n">
+      <x:c r="U25" s="67" t="n">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="V25" s="61" t="str">
+      <x:c r="V25" s="67" t="str">
         <x:v>CARE</x:v>
       </x:c>
     </x:row>
     <x:row r="26">
-      <x:c r="B26" s="61" t="str">
+      <x:c r="B26" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C26" s="61" t="str">
+      <x:c r="C26" s="67" t="str">
         <x:v>S31662</x:v>
       </x:c>
-      <x:c r="D26" s="61" t="str">
+      <x:c r="D26" s="67" t="str">
         <x:v>Chan Kit</x:v>
       </x:c>
-      <x:c r="E26" s="61" t="str">
+      <x:c r="E26" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F26" s="61" t="str">
+      <x:c r="F26" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G26" s="61" t="str">
+      <x:c r="G26" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H26" s="61" t="str">
+      <x:c r="H26" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I26" s="63" t="d">
+      <x:c r="I26" s="69" t="d">
         <x:v>2019-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J26" s="61" t="n">
-        <x:v>1.2268</x:v>
-      </x:c>
-      <x:c r="K26" s="61" t="str">
+      <x:c r="J26" s="67" t="n">
+        <x:v>1.2295</x:v>
+      </x:c>
+      <x:c r="K26" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L26" s="61" t="str">
+      <x:c r="L26" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M26" s="61" t="str">
+      <x:c r="M26" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N26" s="61" t="n">
+      <x:c r="N26" s="67" t="n">
         <x:v>15000</x:v>
       </x:c>
-      <x:c r="O26" s="61" t="n">
+      <x:c r="O26" s="67" t="n">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="P26" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q26" s="63" t="d">
+      <x:c r="P26" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q26" s="69" t="d">
         <x:v>2019-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R26" s="63" t="d">
+      <x:c r="R26" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S26" s="61" t="str">
+      <x:c r="S26" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T26" s="61" t="str">
+      <x:c r="T26" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U26" s="61" t="n">
+      <x:c r="U26" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V26" s="61" t="str">
+      <x:c r="V26" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="27">
-      <x:c r="B27" s="61" t="str">
+      <x:c r="B27" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C27" s="61" t="str">
+      <x:c r="C27" s="67" t="str">
         <x:v>S31663</x:v>
       </x:c>
-      <x:c r="D27" s="61" t="str">
+      <x:c r="D27" s="67" t="str">
         <x:v>Lee Kit</x:v>
       </x:c>
-      <x:c r="E27" s="61" t="str">
+      <x:c r="E27" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F27" s="61" t="str">
+      <x:c r="F27" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G27" s="61" t="str">
+      <x:c r="G27" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H27" s="61" t="str">
+      <x:c r="H27" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I27" s="63" t="d">
+      <x:c r="I27" s="69" t="d">
         <x:v>2019-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J27" s="61" t="n">
-        <x:v>1.2268</x:v>
-      </x:c>
-      <x:c r="K27" s="61" t="str">
+      <x:c r="J27" s="67" t="n">
+        <x:v>1.2295</x:v>
+      </x:c>
+      <x:c r="K27" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L27" s="61" t="str">
+      <x:c r="L27" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M27" s="61" t="str">
+      <x:c r="M27" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N27" s="61" t="n">
+      <x:c r="N27" s="67" t="n">
         <x:v>20000</x:v>
       </x:c>
-      <x:c r="O27" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P27" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q27" s="63" t="d">
+      <x:c r="O27" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P27" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q27" s="69" t="d">
         <x:v>2019-03-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R27" s="63" t="d">
+      <x:c r="R27" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S27" s="61" t="str">
+      <x:c r="S27" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T27" s="61" t="str">
+      <x:c r="T27" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U27" s="61" t="n">
+      <x:c r="U27" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V27" s="61" t="str">
+      <x:c r="V27" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="28">
-      <x:c r="B28" s="61" t="str">
+      <x:c r="B28" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C28" s="61" t="str">
+      <x:c r="C28" s="67" t="str">
         <x:v>S31664</x:v>
       </x:c>
-      <x:c r="D28" s="61" t="str">
+      <x:c r="D28" s="67" t="str">
         <x:v>Staff A</x:v>
       </x:c>
-      <x:c r="E28" s="61" t="str">
+      <x:c r="E28" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F28" s="61" t="str">
+      <x:c r="F28" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G28" s="61" t="str">
+      <x:c r="G28" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H28" s="61" t="str">
+      <x:c r="H28" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I28" s="63" t="d">
+      <x:c r="I28" s="69" t="d">
         <x:v>2004-08-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J28" s="61" t="n">
-        <x:v>15.6448</x:v>
-      </x:c>
-      <x:c r="K28" s="61" t="str">
+      <x:c r="J28" s="67" t="n">
+        <x:v>15.6475</x:v>
+      </x:c>
+      <x:c r="K28" s="67" t="str">
         <x:v>AL17</x:v>
       </x:c>
-      <x:c r="L28" s="61" t="str">
+      <x:c r="L28" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M28" s="61" t="str">
+      <x:c r="M28" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N28" s="61" t="n">
+      <x:c r="N28" s="67" t="n">
         <x:v>62585</x:v>
       </x:c>
-      <x:c r="O28" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P28" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q28" s="63" t="d">
+      <x:c r="O28" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P28" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q28" s="69" t="d">
         <x:v>2018-04-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R28" s="63" t="d">
+      <x:c r="R28" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S28" s="61" t="str">
+      <x:c r="S28" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T28" s="61" t="str">
+      <x:c r="T28" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U28" s="61" t="n">
+      <x:c r="U28" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V28" s="61" t="str">
+      <x:c r="V28" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="29">
-      <x:c r="B29" s="61" t="str">
+      <x:c r="B29" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C29" s="61" t="str">
+      <x:c r="C29" s="67" t="str">
         <x:v>S31665</x:v>
       </x:c>
-      <x:c r="D29" s="61" t="str">
+      <x:c r="D29" s="67" t="str">
         <x:v>Staff B</x:v>
       </x:c>
-      <x:c r="E29" s="61" t="str">
+      <x:c r="E29" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F29" s="61" t="str">
+      <x:c r="F29" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G29" s="61" t="str">
+      <x:c r="G29" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H29" s="61" t="str">
+      <x:c r="H29" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I29" s="63" t="d">
+      <x:c r="I29" s="69" t="d">
         <x:v>2017-08-17T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J29" s="61" t="n">
-        <x:v>2.6038</x:v>
-      </x:c>
-      <x:c r="K29" s="61" t="str">
+      <x:c r="J29" s="67" t="n">
+        <x:v>2.6066</x:v>
+      </x:c>
+      <x:c r="K29" s="67" t="str">
         <x:v>AL21</x:v>
       </x:c>
-      <x:c r="L29" s="61" t="str">
+      <x:c r="L29" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M29" s="61" t="str">
+      <x:c r="M29" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N29" s="61" t="n">
+      <x:c r="N29" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O29" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P29" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q29" s="63" t="d">
+      <x:c r="O29" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P29" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q29" s="69" t="d">
         <x:v>2018-09-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R29" s="63" t="d">
+      <x:c r="R29" s="69" t="d">
         <x:v>2020-12-31T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S29" s="61" t="str">
+      <x:c r="S29" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T29" s="61" t="str">
+      <x:c r="T29" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U29" s="61" t="n">
+      <x:c r="U29" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V29" s="61" t="str">
+      <x:c r="V29" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="30">
-      <x:c r="B30" s="61" t="str">
+      <x:c r="B30" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C30" s="61" t="str">
+      <x:c r="C30" s="67" t="str">
         <x:v>S31666</x:v>
       </x:c>
-      <x:c r="D30" s="61" t="str">
+      <x:c r="D30" s="67" t="str">
         <x:v>Staff Y</x:v>
       </x:c>
-      <x:c r="E30" s="61" t="str">
+      <x:c r="E30" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F30" s="61" t="str">
+      <x:c r="F30" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G30" s="61" t="str">
+      <x:c r="G30" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H30" s="61" t="str">
+      <x:c r="H30" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I30" s="63" t="d">
+      <x:c r="I30" s="69" t="d">
         <x:v>2018-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J30" s="61" t="n">
-        <x:v>2.2268</x:v>
-      </x:c>
-      <x:c r="K30" s="61" t="str">
+      <x:c r="J30" s="67" t="n">
+        <x:v>2.2295</x:v>
+      </x:c>
+      <x:c r="K30" s="67" t="str">
         <x:v>AL18A</x:v>
       </x:c>
-      <x:c r="L30" s="61" t="str">
+      <x:c r="L30" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M30" s="61" t="str">
+      <x:c r="M30" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N30" s="61" t="n">
+      <x:c r="N30" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O30" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P30" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q30" s="63" t="d">
+      <x:c r="O30" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P30" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q30" s="69" t="d">
         <x:v>2018-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R30" s="63" t="d">
+      <x:c r="R30" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S30" s="61" t="str">
+      <x:c r="S30" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T30" s="61" t="str">
+      <x:c r="T30" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U30" s="61" t="n">
+      <x:c r="U30" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V30" s="61" t="str">
+      <x:c r="V30" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="31">
-      <x:c r="B31" s="61" t="str">
+      <x:c r="B31" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C31" s="61" t="str">
+      <x:c r="C31" s="67" t="str">
         <x:v>S31667</x:v>
       </x:c>
-      <x:c r="D31" s="61" t="str">
+      <x:c r="D31" s="67" t="str">
         <x:v>Staff D</x:v>
       </x:c>
-      <x:c r="E31" s="61" t="str">
+      <x:c r="E31" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F31" s="61" t="str">
+      <x:c r="F31" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G31" s="61" t="str">
+      <x:c r="G31" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H31" s="61" t="str">
+      <x:c r="H31" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I31" s="63" t="d">
+      <x:c r="I31" s="69" t="d">
         <x:v>2019-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J31" s="61" t="n">
-        <x:v>1.2268</x:v>
-      </x:c>
-      <x:c r="K31" s="61" t="str">
+      <x:c r="J31" s="67" t="n">
+        <x:v>1.2295</x:v>
+      </x:c>
+      <x:c r="K31" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L31" s="61" t="str">
+      <x:c r="L31" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M31" s="61" t="str">
+      <x:c r="M31" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N31" s="61" t="n">
+      <x:c r="N31" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O31" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P31" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q31" s="63" t="d">
+      <x:c r="O31" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P31" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q31" s="69" t="d">
         <x:v>2019-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R31" s="63" t="d">
+      <x:c r="R31" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S31" s="61" t="str">
+      <x:c r="S31" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T31" s="61" t="str">
+      <x:c r="T31" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U31" s="61" t="n">
+      <x:c r="U31" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V31" s="61" t="str">
+      <x:c r="V31" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="32">
-      <x:c r="B32" s="61" t="str">
+      <x:c r="B32" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C32" s="61" t="str">
+      <x:c r="C32" s="67" t="str">
         <x:v>S31670</x:v>
       </x:c>
-      <x:c r="D32" s="61" t="str">
+      <x:c r="D32" s="67" t="str">
         <x:v>Staff F</x:v>
       </x:c>
-      <x:c r="E32" s="61" t="str">
+      <x:c r="E32" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F32" s="61" t="str">
+      <x:c r="F32" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G32" s="61" t="str">
+      <x:c r="G32" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H32" s="61" t="str">
+      <x:c r="H32" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I32" s="63" t="d">
+      <x:c r="I32" s="69" t="d">
         <x:v>2018-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J32" s="61" t="n">
-        <x:v>2.2268</x:v>
-      </x:c>
-      <x:c r="K32" s="61" t="str">
+      <x:c r="J32" s="67" t="n">
+        <x:v>2.2295</x:v>
+      </x:c>
+      <x:c r="K32" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L32" s="61" t="str">
+      <x:c r="L32" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M32" s="61" t="str">
+      <x:c r="M32" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N32" s="61" t="n">
+      <x:c r="N32" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O32" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P32" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q32" s="63" t="d">
+      <x:c r="O32" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P32" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q32" s="69" t="d">
         <x:v>2018-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R32" s="63" t="d">
+      <x:c r="R32" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S32" s="61" t="str">
+      <x:c r="S32" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T32" s="61" t="str">
+      <x:c r="T32" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U32" s="61" t="n">
+      <x:c r="U32" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V32" s="61" t="str">
+      <x:c r="V32" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="33">
-      <x:c r="B33" s="61" t="str">
+      <x:c r="B33" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C33" s="61" t="str">
+      <x:c r="C33" s="67" t="str">
         <x:v>S31671</x:v>
       </x:c>
-      <x:c r="D33" s="61" t="str">
+      <x:c r="D33" s="67" t="str">
         <x:v>Staff CA</x:v>
       </x:c>
-      <x:c r="E33" s="61" t="str">
+      <x:c r="E33" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F33" s="61" t="str">
+      <x:c r="F33" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G33" s="61" t="str">
+      <x:c r="G33" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H33" s="61" t="str">
+      <x:c r="H33" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I33" s="63" t="d">
+      <x:c r="I33" s="69" t="d">
         <x:v>2017-10-17T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J33" s="61" t="n">
-        <x:v>2.4372</x:v>
-      </x:c>
-      <x:c r="K33" s="61" t="str">
+      <x:c r="J33" s="67" t="n">
+        <x:v>2.4399</x:v>
+      </x:c>
+      <x:c r="K33" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L33" s="61" t="str">
+      <x:c r="L33" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M33" s="61" t="str">
+      <x:c r="M33" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N33" s="61" t="n">
+      <x:c r="N33" s="67" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="O33" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P33" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q33" s="63" t="d">
+      <x:c r="O33" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P33" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q33" s="69" t="d">
         <x:v>2020-08-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R33" s="63" t="d">
+      <x:c r="R33" s="69" t="d">
         <x:v>2021-10-17T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S33" s="61" t="str">
+      <x:c r="S33" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T33" s="61" t="str">
+      <x:c r="T33" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U33" s="61" t="n">
+      <x:c r="U33" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V33" s="61" t="str">
+      <x:c r="V33" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="34">
-      <x:c r="B34" s="61" t="str">
+      <x:c r="B34" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C34" s="61" t="str">
+      <x:c r="C34" s="67" t="str">
         <x:v>S31672</x:v>
       </x:c>
-      <x:c r="D34" s="61" t="str">
+      <x:c r="D34" s="67" t="str">
         <x:v>Staff G</x:v>
       </x:c>
-      <x:c r="E34" s="61" t="str">
+      <x:c r="E34" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F34" s="61" t="str">
+      <x:c r="F34" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G34" s="61" t="str">
+      <x:c r="G34" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H34" s="61" t="str">
+      <x:c r="H34" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I34" s="63" t="d">
+      <x:c r="I34" s="69" t="d">
         <x:v>2017-03-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J34" s="61" t="n">
-        <x:v>3.0656</x:v>
-      </x:c>
-      <x:c r="K34" s="61" t="str">
+      <x:c r="J34" s="67" t="n">
+        <x:v>3.0683</x:v>
+      </x:c>
+      <x:c r="K34" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L34" s="61" t="str">
+      <x:c r="L34" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M34" s="61" t="str">
+      <x:c r="M34" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N34" s="61" t="n">
+      <x:c r="N34" s="67" t="n">
         <x:v>6635</x:v>
       </x:c>
-      <x:c r="O34" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P34" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q34" s="63" t="d">
+      <x:c r="O34" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P34" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q34" s="69" t="d">
         <x:v>2017-08-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R34" s="63" t="d">
+      <x:c r="R34" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S34" s="61" t="str">
+      <x:c r="S34" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T34" s="61" t="str">
+      <x:c r="T34" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U34" s="61" t="n">
+      <x:c r="U34" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V34" s="61" t="str">
+      <x:c r="V34" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="35">
-      <x:c r="B35" s="61" t="str">
+      <x:c r="B35" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C35" s="61" t="str">
+      <x:c r="C35" s="67" t="str">
         <x:v>S31673</x:v>
       </x:c>
-      <x:c r="D35" s="61" t="str">
+      <x:c r="D35" s="67" t="str">
         <x:v>Staff AA</x:v>
       </x:c>
-      <x:c r="E35" s="61" t="str">
+      <x:c r="E35" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F35" s="61" t="str">
+      <x:c r="F35" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G35" s="61" t="str">
+      <x:c r="G35" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H35" s="61" t="str">
+      <x:c r="H35" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I35" s="63" t="d">
+      <x:c r="I35" s="69" t="d">
         <x:v>2018-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J35" s="61" t="n">
-        <x:v>2.2268</x:v>
-      </x:c>
-      <x:c r="K35" s="61" t="str">
+      <x:c r="J35" s="67" t="n">
+        <x:v>2.2295</x:v>
+      </x:c>
+      <x:c r="K35" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L35" s="61" t="str">
+      <x:c r="L35" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M35" s="61" t="str">
+      <x:c r="M35" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N35" s="61" t="n">
+      <x:c r="N35" s="67" t="n">
         <x:v>62585</x:v>
       </x:c>
-      <x:c r="O35" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P35" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q35" s="63" t="d">
+      <x:c r="O35" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P35" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q35" s="69" t="d">
         <x:v>2018-10-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R35" s="63" t="d">
+      <x:c r="R35" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S35" s="61" t="str">
+      <x:c r="S35" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T35" s="61" t="str">
+      <x:c r="T35" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U35" s="61" t="n">
+      <x:c r="U35" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V35" s="61" t="str">
+      <x:c r="V35" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="36">
-      <x:c r="B36" s="61" t="str">
+      <x:c r="B36" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C36" s="61" t="str">
+      <x:c r="C36" s="67" t="str">
         <x:v>S31674</x:v>
       </x:c>
-      <x:c r="D36" s="61" t="str">
+      <x:c r="D36" s="67" t="str">
         <x:v>Staff BB</x:v>
       </x:c>
-      <x:c r="E36" s="61" t="str">
+      <x:c r="E36" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F36" s="61" t="str">
+      <x:c r="F36" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G36" s="61" t="str">
+      <x:c r="G36" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H36" s="61" t="str">
+      <x:c r="H36" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I36" s="63" t="d">
+      <x:c r="I36" s="69" t="d">
         <x:v>2018-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J36" s="61" t="n">
-        <x:v>2.2268</x:v>
-      </x:c>
-      <x:c r="K36" s="61" t="str">
+      <x:c r="J36" s="67" t="n">
+        <x:v>2.2295</x:v>
+      </x:c>
+      <x:c r="K36" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L36" s="61" t="str">
+      <x:c r="L36" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M36" s="61" t="str">
+      <x:c r="M36" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N36" s="61" t="n">
+      <x:c r="N36" s="67" t="n">
         <x:v>68500</x:v>
       </x:c>
-      <x:c r="O36" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P36" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q36" s="63" t="d">
+      <x:c r="O36" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P36" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q36" s="69" t="d">
         <x:v>2019-02-18T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R36" s="63" t="d">
+      <x:c r="R36" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S36" s="61" t="str">
+      <x:c r="S36" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T36" s="61" t="str">
+      <x:c r="T36" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U36" s="61" t="n">
+      <x:c r="U36" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V36" s="61" t="str">
+      <x:c r="V36" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="37">
-      <x:c r="B37" s="61" t="str">
+      <x:c r="B37" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C37" s="61" t="str">
+      <x:c r="C37" s="67" t="str">
         <x:v>S31675</x:v>
       </x:c>
-      <x:c r="D37" s="61" t="str">
+      <x:c r="D37" s="67" t="str">
         <x:v>Staff M</x:v>
       </x:c>
-      <x:c r="E37" s="61" t="str">
+      <x:c r="E37" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F37" s="61" t="str">
+      <x:c r="F37" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G37" s="61" t="str">
+      <x:c r="G37" s="67" t="str">
         <x:v>HEALTH WORKERS</x:v>
       </x:c>
-      <x:c r="H37" s="61" t="str">
+      <x:c r="H37" s="67" t="str">
         <x:v>保健員</x:v>
       </x:c>
-      <x:c r="I37" s="63" t="d">
+      <x:c r="I37" s="69" t="d">
         <x:v>2017-08-17T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J37" s="61" t="n">
-        <x:v>2.6038</x:v>
-      </x:c>
-      <x:c r="K37" s="61" t="str">
+      <x:c r="J37" s="67" t="n">
+        <x:v>2.6066</x:v>
+      </x:c>
+      <x:c r="K37" s="67" t="str">
         <x:v>AL18</x:v>
       </x:c>
-      <x:c r="L37" s="61" t="str">
+      <x:c r="L37" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M37" s="61" t="str">
+      <x:c r="M37" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N37" s="61" t="n">
+      <x:c r="N37" s="67" t="n">
         <x:v>15000</x:v>
       </x:c>
-      <x:c r="O37" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P37" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q37" s="63" t="d">
+      <x:c r="O37" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P37" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q37" s="69" t="d">
         <x:v>2018-09-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R37" s="63" t="d">
+      <x:c r="R37" s="69" t="d">
         <x:v>2020-08-17T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S37" s="61" t="str">
+      <x:c r="S37" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T37" s="61" t="str">
+      <x:c r="T37" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U37" s="61" t="n">
+      <x:c r="U37" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V37" s="61" t="str">
+      <x:c r="V37" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="38">
-      <x:c r="B38" s="61" t="str">
+      <x:c r="B38" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C38" s="61" t="str">
+      <x:c r="C38" s="67" t="str">
         <x:v>S31614</x:v>
       </x:c>
-      <x:c r="D38" s="61" t="str">
+      <x:c r="D38" s="67" t="str">
         <x:v>Lau Wah</x:v>
       </x:c>
-      <x:c r="E38" s="61" t="str">
+      <x:c r="E38" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F38" s="61" t="str">
+      <x:c r="F38" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G38" s="61" t="str">
+      <x:c r="G38" s="67" t="str">
         <x:v>HW2</x:v>
       </x:c>
-      <x:c r="H38" s="61" t="str">
+      <x:c r="H38" s="67" t="str">
         <x:v>福利服務助理</x:v>
       </x:c>
-      <x:c r="I38" s="63" t="d">
+      <x:c r="I38" s="69" t="d">
         <x:v>2016-01-04T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J38" s="61" t="n">
-        <x:v>4.2186</x:v>
-      </x:c>
-      <x:c r="K38" s="61" t="str">
+      <x:c r="J38" s="67" t="n">
+        <x:v>4.2213</x:v>
+      </x:c>
+      <x:c r="K38" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L38" s="61" t="str">
+      <x:c r="L38" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M38" s="61" t="str">
+      <x:c r="M38" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N38" s="61" t="n">
+      <x:c r="N38" s="67" t="n">
         <x:v>60</x:v>
       </x:c>
-      <x:c r="O38" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P38" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q38" s="63" t="d">
+      <x:c r="O38" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P38" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q38" s="69" t="d">
         <x:v>2017-08-15T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R38" s="63" t="d">
+      <x:c r="R38" s="69" t="d">
         <x:v>2053-05-25T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S38" s="61" t="str">
+      <x:c r="S38" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T38" s="61" t="str">
+      <x:c r="T38" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U38" s="61" t="n">
+      <x:c r="U38" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V38" s="61" t="str">
+      <x:c r="V38" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="39">
-      <x:c r="B39" s="61" t="str">
+      <x:c r="B39" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C39" s="61" t="str">
+      <x:c r="C39" s="67" t="str">
         <x:v>S31649</x:v>
       </x:c>
-      <x:c r="D39" s="61" t="str">
+      <x:c r="D39" s="67" t="str">
         <x:v>Chan Chi Man</x:v>
       </x:c>
-      <x:c r="E39" s="61" t="str">
+      <x:c r="E39" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F39" s="61" t="str">
+      <x:c r="F39" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G39" s="61" t="str">
+      <x:c r="G39" s="67" t="str">
         <x:v>HW2</x:v>
       </x:c>
-      <x:c r="H39" s="61" t="str">
+      <x:c r="H39" s="67" t="str">
         <x:v>福利服務助理</x:v>
       </x:c>
-      <x:c r="I39" s="63" t="d">
+      <x:c r="I39" s="69" t="d">
         <x:v>2018-03-08T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J39" s="61" t="n">
-        <x:v>2.0464</x:v>
-      </x:c>
-      <x:c r="K39" s="61" t="str">
+      <x:c r="J39" s="67" t="n">
+        <x:v>2.0492</x:v>
+      </x:c>
+      <x:c r="K39" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L39" s="61" t="str">
+      <x:c r="L39" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M39" s="61" t="str">
+      <x:c r="M39" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N39" s="61" t="n">
+      <x:c r="N39" s="67" t="n">
         <x:v>20650</x:v>
       </x:c>
-      <x:c r="O39" s="61" t="n">
+      <x:c r="O39" s="67" t="n">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="P39" s="61" t="str">
+      <x:c r="P39" s="67" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="Q39" s="63" t="d">
+      <x:c r="Q39" s="69" t="d">
         <x:v>2018-03-08T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R39" s="63" t="d">
+      <x:c r="R39" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S39" s="61" t="str">
+      <x:c r="S39" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T39" s="61" t="str">
+      <x:c r="T39" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U39" s="61" t="n">
+      <x:c r="U39" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V39" s="61" t="str">
+      <x:c r="V39" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="40">
-      <x:c r="B40" s="61" t="str">
+      <x:c r="B40" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C40" s="61" t="str">
+      <x:c r="C40" s="67" t="str">
         <x:v>S31660</x:v>
       </x:c>
-      <x:c r="D40" s="61" t="str">
+      <x:c r="D40" s="67" t="str">
         <x:v>Chan King</x:v>
       </x:c>
-      <x:c r="E40" s="61" t="str">
+      <x:c r="E40" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F40" s="61" t="str">
+      <x:c r="F40" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G40" s="61" t="str">
+      <x:c r="G40" s="67" t="str">
         <x:v>HW2</x:v>
       </x:c>
-      <x:c r="H40" s="61" t="str">
+      <x:c r="H40" s="67" t="str">
         <x:v>福利服務助理</x:v>
       </x:c>
-      <x:c r="I40" s="63" t="d">
+      <x:c r="I40" s="69" t="d">
         <x:v>2018-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J40" s="61" t="n">
-        <x:v>2.2268</x:v>
-      </x:c>
-      <x:c r="K40" s="61" t="str">
+      <x:c r="J40" s="67" t="n">
+        <x:v>2.2295</x:v>
+      </x:c>
+      <x:c r="K40" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L40" s="61" t="str">
+      <x:c r="L40" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M40" s="61" t="str">
+      <x:c r="M40" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N40" s="61" t="n">
+      <x:c r="N40" s="67" t="n">
         <x:v>16000</x:v>
       </x:c>
-      <x:c r="O40" s="61" t="n">
+      <x:c r="O40" s="67" t="n">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="P40" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q40" s="63" t="d">
+      <x:c r="P40" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q40" s="69" t="d">
         <x:v>2018-12-14T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R40" s="63" t="d">
+      <x:c r="R40" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S40" s="61" t="str">
+      <x:c r="S40" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T40" s="61" t="str">
+      <x:c r="T40" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U40" s="61" t="n">
+      <x:c r="U40" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V40" s="61" t="str">
+      <x:c r="V40" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="41">
-      <x:c r="B41" s="61" t="str">
+      <x:c r="B41" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C41" s="61" t="str">
+      <x:c r="C41" s="67" t="str">
         <x:v>S31633</x:v>
       </x:c>
-      <x:c r="D41" s="61" t="str">
+      <x:c r="D41" s="67" t="str">
         <x:v>WONG Ka Wai</x:v>
       </x:c>
-      <x:c r="E41" s="61" t="str">
+      <x:c r="E41" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F41" s="61" t="str">
+      <x:c r="F41" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G41" s="61" t="str">
+      <x:c r="G41" s="67" t="str">
         <x:v>MISC</x:v>
       </x:c>
-      <x:c r="H41" s="61" t="str">
+      <x:c r="H41" s="67" t="str">
         <x:v>MISC 打雜</x:v>
       </x:c>
-      <x:c r="I41" s="63" t="d">
+      <x:c r="I41" s="69" t="d">
         <x:v>2016-09-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J41" s="61" t="n">
-        <x:v>3.5628</x:v>
-      </x:c>
-      <x:c r="K41" s="61" t="str">
+      <x:c r="J41" s="67" t="n">
+        <x:v>3.5656</x:v>
+      </x:c>
+      <x:c r="K41" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L41" s="61" t="str">
+      <x:c r="L41" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M41" s="61" t="str">
+      <x:c r="M41" s="67" t="str">
         <x:v>Daily</x:v>
       </x:c>
-      <x:c r="N41" s="61" t="n">
+      <x:c r="N41" s="67" t="n">
         <x:v>200</x:v>
       </x:c>
-      <x:c r="O41" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P41" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q41" s="63" t="d">
+      <x:c r="O41" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P41" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q41" s="69" t="d">
         <x:v>2018-09-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R41" s="63" t="d">
+      <x:c r="R41" s="69" t="d">
         <x:v>2061-05-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S41" s="61" t="str">
+      <x:c r="S41" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T41" s="61" t="str">
+      <x:c r="T41" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U41" s="61" t="n">
+      <x:c r="U41" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V41" s="61" t="str">
+      <x:c r="V41" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="42">
-      <x:c r="B42" s="61" t="str">
+      <x:c r="B42" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C42" s="61" t="str">
+      <x:c r="C42" s="67" t="str">
         <x:v>S31640</x:v>
       </x:c>
-      <x:c r="D42" s="61" t="str">
+      <x:c r="D42" s="67" t="str">
         <x:v>Lau Li Chun</x:v>
       </x:c>
-      <x:c r="E42" s="61" t="str">
+      <x:c r="E42" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F42" s="61" t="str">
+      <x:c r="F42" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G42" s="61" t="str">
+      <x:c r="G42" s="67" t="str">
         <x:v>MISC</x:v>
       </x:c>
-      <x:c r="H42" s="61" t="str">
+      <x:c r="H42" s="67" t="str">
         <x:v>MISC 打雜</x:v>
       </x:c>
-      <x:c r="I42" s="63" t="d">
+      <x:c r="I42" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J42" s="61" t="n">
-        <x:v>2.224</x:v>
-      </x:c>
-      <x:c r="K42" s="61" t="str">
+      <x:c r="J42" s="67" t="n">
+        <x:v>2.2268</x:v>
+      </x:c>
+      <x:c r="K42" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L42" s="61" t="str">
+      <x:c r="L42" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M42" s="61" t="str">
+      <x:c r="M42" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N42" s="61" t="n">
+      <x:c r="N42" s="67" t="n">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="O42" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P42" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q42" s="63" t="d">
+      <x:c r="O42" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P42" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q42" s="69" t="d">
         <x:v>2018-01-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R42" s="63" t="d">
+      <x:c r="R42" s="69" t="d">
         <x:v>2041-04-02T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S42" s="61" t="str">
+      <x:c r="S42" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T42" s="61" t="str">
+      <x:c r="T42" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U42" s="61" t="n">
+      <x:c r="U42" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V42" s="61" t="str">
+      <x:c r="V42" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="43">
-      <x:c r="B43" s="61" t="str">
+      <x:c r="B43" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C43" s="61" t="str">
+      <x:c r="C43" s="67" t="str">
         <x:v>S31651</x:v>
       </x:c>
-      <x:c r="D43" s="61" t="str">
+      <x:c r="D43" s="67" t="str">
         <x:v>Chan Tai Man, Peter</x:v>
       </x:c>
-      <x:c r="E43" s="61" t="str">
+      <x:c r="E43" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F43" s="61" t="str">
+      <x:c r="F43" s="67" t="str">
         <x:v>General Staff 普通員工</x:v>
       </x:c>
-      <x:c r="G43" s="61" t="str">
+      <x:c r="G43" s="67" t="str">
         <x:v>PE</x:v>
       </x:c>
-      <x:c r="H43" s="61" t="str">
+      <x:c r="H43" s="67" t="str">
         <x:v>Project Executive</x:v>
       </x:c>
-      <x:c r="I43" s="63" t="d">
+      <x:c r="I43" s="69" t="d">
         <x:v>2016-11-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J43" s="61" t="n">
-        <x:v>3.3716</x:v>
-      </x:c>
-      <x:c r="K43" s="61" t="str">
+      <x:c r="J43" s="67" t="n">
+        <x:v>3.3743</x:v>
+      </x:c>
+      <x:c r="K43" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L43" s="61" t="str">
+      <x:c r="L43" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M43" s="61" t="str">
+      <x:c r="M43" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N43" s="61" t="n">
+      <x:c r="N43" s="67" t="n">
         <x:v>30320</x:v>
       </x:c>
-      <x:c r="O43" s="61" t="n">
+      <x:c r="O43" s="67" t="n">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="P43" s="61" t="str">
+      <x:c r="P43" s="67" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="Q43" s="63" t="d">
+      <x:c r="Q43" s="69" t="d">
         <x:v>2017-11-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R43" s="63" t="d">
+      <x:c r="R43" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S43" s="61" t="str">
+      <x:c r="S43" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T43" s="61" t="str">
+      <x:c r="T43" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U43" s="61" t="n">
+      <x:c r="U43" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V43" s="61" t="str">
+      <x:c r="V43" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="44">
-      <x:c r="B44" s="61" t="str">
+      <x:c r="B44" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C44" s="61" t="str">
+      <x:c r="C44" s="67" t="str">
         <x:v>S31652</x:v>
       </x:c>
-      <x:c r="D44" s="61" t="str">
+      <x:c r="D44" s="67" t="str">
         <x:v>Wong Siu Ming, John</x:v>
       </x:c>
-      <x:c r="E44" s="61" t="str">
+      <x:c r="E44" s="67" t="str">
         <x:v>Unit B</x:v>
       </x:c>
-      <x:c r="F44" s="61" t="str">
+      <x:c r="F44" s="67" t="str">
         <x:v>HR Admin</x:v>
       </x:c>
-      <x:c r="G44" s="61" t="str">
+      <x:c r="G44" s="67" t="str">
         <x:v>HRADMIN</x:v>
       </x:c>
-      <x:c r="H44" s="61" t="str">
+      <x:c r="H44" s="67" t="str">
         <x:v>HR Admin</x:v>
       </x:c>
-      <x:c r="I44" s="63" t="d">
+      <x:c r="I44" s="69" t="d">
         <x:v>2015-02-04T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J44" s="61" t="n">
-        <x:v>5.1339</x:v>
-      </x:c>
-      <x:c r="K44" s="61" t="str">
+      <x:c r="J44" s="67" t="n">
+        <x:v>5.1366</x:v>
+      </x:c>
+      <x:c r="K44" s="67" t="str">
         <x:v>AL07</x:v>
       </x:c>
-      <x:c r="L44" s="61" t="str">
+      <x:c r="L44" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M44" s="61" t="str">
+      <x:c r="M44" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N44" s="61" t="n">
+      <x:c r="N44" s="67" t="n">
         <x:v>40300</x:v>
       </x:c>
-      <x:c r="O44" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P44" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q44" s="63" t="d">
+      <x:c r="O44" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P44" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q44" s="69" t="d">
         <x:v>2015-02-04T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R44" s="63" t="d">
+      <x:c r="R44" s="69" t="d">
         <x:v>2047-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S44" s="61" t="str">
+      <x:c r="S44" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T44" s="61" t="str">
+      <x:c r="T44" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U44" s="61" t="n">
+      <x:c r="U44" s="67" t="n">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="V44" s="61" t="str">
+      <x:c r="V44" s="67" t="str">
         <x:v>User</x:v>
       </x:c>
     </x:row>
     <x:row r="45">
-      <x:c r="B45" s="61" t="str">
+      <x:c r="B45" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C45" s="61" t="str">
+      <x:c r="C45" s="67" t="str">
         <x:v>S31658</x:v>
       </x:c>
-      <x:c r="D45" s="61" t="str">
+      <x:c r="D45" s="67" t="str">
         <x:v>Leung Mai Mai</x:v>
       </x:c>
-      <x:c r="E45" s="61" t="str">
+      <x:c r="E45" s="67" t="str">
         <x:v>Unit B</x:v>
       </x:c>
-      <x:c r="F45" s="61" t="str">
+      <x:c r="F45" s="67" t="str">
         <x:v>HR Admin</x:v>
       </x:c>
-      <x:c r="G45" s="61" t="str">
+      <x:c r="G45" s="67" t="str">
         <x:v>HRADMIN</x:v>
       </x:c>
-      <x:c r="H45" s="61" t="str">
+      <x:c r="H45" s="67" t="str">
         <x:v>HR Admin</x:v>
       </x:c>
-      <x:c r="I45" s="63" t="d">
+      <x:c r="I45" s="69" t="d">
         <x:v>2010-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J45" s="61" t="n">
-        <x:v>9.3962</x:v>
-      </x:c>
-      <x:c r="K45" s="61" t="str">
+      <x:c r="J45" s="67" t="n">
+        <x:v>9.3989</x:v>
+      </x:c>
+      <x:c r="K45" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L45" s="61" t="str">
+      <x:c r="L45" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M45" s="61" t="str">
+      <x:c r="M45" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N45" s="61" t="n">
+      <x:c r="N45" s="67" t="n">
         <x:v>41000</x:v>
       </x:c>
-      <x:c r="O45" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P45" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q45" s="63" t="d">
+      <x:c r="O45" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P45" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q45" s="69" t="d">
         <x:v>2019-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R45" s="63" t="d">
+      <x:c r="R45" s="69" t="d">
         <x:v>2020-05-31T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S45" s="61" t="str">
+      <x:c r="S45" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T45" s="61" t="str">
+      <x:c r="T45" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U45" s="61" t="n">
+      <x:c r="U45" s="67" t="n">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="V45" s="61" t="str">
+      <x:c r="V45" s="67" t="str">
         <x:v>General Office</x:v>
       </x:c>
     </x:row>
     <x:row r="46">
-      <x:c r="B46" s="61" t="str">
+      <x:c r="B46" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C46" s="61" t="str">
+      <x:c r="C46" s="67" t="str">
         <x:v>S31659</x:v>
       </x:c>
-      <x:c r="D46" s="61" t="str">
+      <x:c r="D46" s="67" t="str">
         <x:v>Yeung Chau Ha</x:v>
       </x:c>
-      <x:c r="E46" s="61" t="str">
+      <x:c r="E46" s="67" t="str">
         <x:v>Unit B</x:v>
       </x:c>
-      <x:c r="F46" s="61" t="str">
+      <x:c r="F46" s="67" t="str">
         <x:v>HR Admin</x:v>
       </x:c>
-      <x:c r="G46" s="61" t="str">
+      <x:c r="G46" s="67" t="str">
         <x:v>HRADMIN</x:v>
       </x:c>
-      <x:c r="H46" s="61" t="str">
+      <x:c r="H46" s="67" t="str">
         <x:v>HR Admin</x:v>
       </x:c>
-      <x:c r="I46" s="63" t="d">
+      <x:c r="I46" s="69" t="d">
         <x:v>2018-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J46" s="61" t="n">
-        <x:v>1.3962</x:v>
-      </x:c>
-      <x:c r="K46" s="61" t="str">
+      <x:c r="J46" s="67" t="n">
+        <x:v>1.3989</x:v>
+      </x:c>
+      <x:c r="K46" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L46" s="61" t="str">
+      <x:c r="L46" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M46" s="61" t="str">
+      <x:c r="M46" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N46" s="61" t="n">
+      <x:c r="N46" s="67" t="n">
         <x:v>42500</x:v>
       </x:c>
-      <x:c r="O46" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P46" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q46" s="63" t="d">
+      <x:c r="O46" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P46" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q46" s="69" t="d">
         <x:v>2018-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R46" s="63" t="d">
+      <x:c r="R46" s="69" t="d">
         <x:v>2048-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S46" s="61" t="str">
+      <x:c r="S46" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T46" s="61" t="str">
+      <x:c r="T46" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U46" s="61" t="n">
+      <x:c r="U46" s="67" t="n">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="V46" s="61" t="str">
+      <x:c r="V46" s="67" t="str">
         <x:v>General Office</x:v>
       </x:c>
     </x:row>
     <x:row r="47">
-      <x:c r="B47" s="61" t="str">
+      <x:c r="B47" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C47" s="61" t="str">
+      <x:c r="C47" s="67" t="str">
         <x:v>S31613</x:v>
       </x:c>
-      <x:c r="D47" s="61" t="str">
+      <x:c r="D47" s="67" t="str">
         <x:v>Wong Chi Man</x:v>
       </x:c>
-      <x:c r="E47" s="61" t="str">
+      <x:c r="E47" s="67" t="str">
         <x:v>Unit C</x:v>
       </x:c>
-      <x:c r="F47" s="61" t="str">
+      <x:c r="F47" s="67" t="str">
         <x:v>Manager Unit Incharge 经理主管</x:v>
       </x:c>
-      <x:c r="G47" s="61" t="str">
+      <x:c r="G47" s="67" t="str">
         <x:v>ED</x:v>
       </x:c>
-      <x:c r="H47" s="61" t="str">
+      <x:c r="H47" s="67" t="str">
         <x:v>EXECUTIVE DIRECTOR 總幹事</x:v>
       </x:c>
-      <x:c r="I47" s="63" t="d">
+      <x:c r="I47" s="69" t="d">
         <x:v>2016-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J47" s="61" t="n">
-        <x:v>4.2268</x:v>
-      </x:c>
-      <x:c r="K47" s="61" t="str">
+      <x:c r="J47" s="67" t="n">
+        <x:v>4.2295</x:v>
+      </x:c>
+      <x:c r="K47" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L47" s="61" t="str">
+      <x:c r="L47" s="67" t="str">
         <x:v>Bank Holiday</x:v>
       </x:c>
-      <x:c r="M47" s="61" t="str">
+      <x:c r="M47" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N47" s="61" t="n">
+      <x:c r="N47" s="67" t="n">
         <x:v>73700</x:v>
       </x:c>
-      <x:c r="O47" s="61" t="n">
+      <x:c r="O47" s="67" t="n">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="P47" s="61" t="str">
+      <x:c r="P47" s="67" t="str">
         <x:v>MPS</x:v>
       </x:c>
-      <x:c r="Q47" s="63" t="d">
+      <x:c r="Q47" s="69" t="d">
         <x:v>2017-08-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R47" s="63" t="d">
+      <x:c r="R47" s="69" t="d">
         <x:v>2040-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S47" s="61" t="str">
+      <x:c r="S47" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T47" s="61" t="str">
+      <x:c r="T47" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U47" s="61" t="n">
+      <x:c r="U47" s="67" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="V47" s="61" t="str">
+      <x:c r="V47" s="67" t="str">
         <x:v>TST</x:v>
       </x:c>
     </x:row>
     <x:row r="48">
-      <x:c r="B48" s="61" t="str">
+      <x:c r="B48" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C48" s="61" t="str">
+      <x:c r="C48" s="67" t="str">
         <x:v>S31657</x:v>
       </x:c>
-      <x:c r="D48" s="61" t="str">
+      <x:c r="D48" s="67" t="str">
         <x:v>Wong Tai Man</x:v>
       </x:c>
-      <x:c r="E48" s="61" t="str">
+      <x:c r="E48" s="67" t="str">
         <x:v>Unit B</x:v>
       </x:c>
-      <x:c r="F48" s="61" t="str">
+      <x:c r="F48" s="67" t="str">
         <x:v>Manager Unit Incharge 经理主管</x:v>
       </x:c>
-      <x:c r="G48" s="61" t="str">
+      <x:c r="G48" s="67" t="str">
         <x:v>HRM</x:v>
       </x:c>
-      <x:c r="H48" s="61" t="str">
+      <x:c r="H48" s="67" t="str">
         <x:v>HR manager</x:v>
       </x:c>
-      <x:c r="I48" s="63" t="d">
+      <x:c r="I48" s="69" t="d">
         <x:v>2018-11-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J48" s="61" t="n">
-        <x:v>1.3962</x:v>
-      </x:c>
-      <x:c r="K48" s="61" t="str">
+      <x:c r="J48" s="67" t="n">
+        <x:v>1.3989</x:v>
+      </x:c>
+      <x:c r="K48" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L48" s="61" t="str">
+      <x:c r="L48" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M48" s="61" t="str">
+      <x:c r="M48" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N48" s="61" t="n">
+      <x:c r="N48" s="67" t="n">
         <x:v>45000</x:v>
       </x:c>
-      <x:c r="O48" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P48" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q48" s="63" t="d">
+      <x:c r="O48" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P48" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q48" s="69" t="d">
         <x:v>2043-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R48" s="63" t="d">
+      <x:c r="R48" s="69" t="d">
         <x:v>2099-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S48" s="61" t="str">
+      <x:c r="S48" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T48" s="61" t="str">
+      <x:c r="T48" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U48" s="61" t="n">
+      <x:c r="U48" s="67" t="n">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="V48" s="61" t="str">
+      <x:c r="V48" s="67" t="str">
         <x:v>General Office</x:v>
       </x:c>
     </x:row>
     <x:row r="49">
-      <x:c r="B49" s="61" t="str">
+      <x:c r="B49" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C49" s="61" t="str">
+      <x:c r="C49" s="67" t="str">
         <x:v>S31630</x:v>
       </x:c>
-      <x:c r="D49" s="61" t="str">
+      <x:c r="D49" s="67" t="str">
         <x:v>LAM Lai Wo</x:v>
       </x:c>
-      <x:c r="E49" s="61" t="str">
+      <x:c r="E49" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F49" s="61" t="str">
+      <x:c r="F49" s="67" t="str">
         <x:v>Personal Care Worker</x:v>
       </x:c>
-      <x:c r="G49" s="61" t="str">
+      <x:c r="G49" s="67" t="str">
         <x:v>PCW</x:v>
       </x:c>
-      <x:c r="H49" s="61" t="str">
+      <x:c r="H49" s="67" t="str">
         <x:v>護理員 Personal Care  Worker</x:v>
       </x:c>
-      <x:c r="I49" s="63" t="d">
+      <x:c r="I49" s="69" t="d">
         <x:v>2016-09-06T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J49" s="61" t="n">
-        <x:v>3.5492</x:v>
-      </x:c>
-      <x:c r="K49" s="61" t="str">
+      <x:c r="J49" s="67" t="n">
+        <x:v>3.5519</x:v>
+      </x:c>
+      <x:c r="K49" s="67" t="str">
         <x:v>AL14</x:v>
       </x:c>
-      <x:c r="L49" s="61" t="str">
+      <x:c r="L49" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M49" s="61" t="str">
+      <x:c r="M49" s="67" t="str">
         <x:v>Monthly</x:v>
       </x:c>
-      <x:c r="N49" s="61" t="n">
+      <x:c r="N49" s="67" t="n">
         <x:v>15000</x:v>
       </x:c>
-      <x:c r="O49" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P49" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q49" s="63" t="d">
+      <x:c r="O49" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P49" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q49" s="69" t="d">
         <x:v>2016-09-06T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R49" s="63" t="d">
+      <x:c r="R49" s="69" t="d">
         <x:v>2033-09-04T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S49" s="61" t="str">
+      <x:c r="S49" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T49" s="61" t="str">
+      <x:c r="T49" s="67" t="str">
         <x:v>No</x:v>
       </x:c>
-      <x:c r="U49" s="61" t="n">
+      <x:c r="U49" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V49" s="61" t="str">
+      <x:c r="V49" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="50">
-      <x:c r="B50" s="61" t="str">
+      <x:c r="B50" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C50" s="61" t="str">
+      <x:c r="C50" s="67" t="str">
         <x:v>S31631</x:v>
       </x:c>
-      <x:c r="D50" s="61" t="str">
+      <x:c r="D50" s="67" t="str">
         <x:v>Lau Kin Fai</x:v>
       </x:c>
-      <x:c r="E50" s="61" t="str">
+      <x:c r="E50" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F50" s="61" t="str">
+      <x:c r="F50" s="67" t="str">
         <x:v>Personal Care Worker</x:v>
       </x:c>
-      <x:c r="G50" s="61" t="str">
+      <x:c r="G50" s="67" t="str">
         <x:v>PCW</x:v>
       </x:c>
-      <x:c r="H50" s="61" t="str">
+      <x:c r="H50" s="67" t="str">
         <x:v>護理員 Personal Care  Worker</x:v>
       </x:c>
-      <x:c r="I50" s="63" t="d">
+      <x:c r="I50" s="69" t="d">
         <x:v>2016-09-06T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J50" s="61" t="n">
-        <x:v>3.5492</x:v>
-      </x:c>
-      <x:c r="K50" s="61" t="str">
+      <x:c r="J50" s="67" t="n">
+        <x:v>3.5519</x:v>
+      </x:c>
+      <x:c r="K50" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L50" s="61" t="str">
+      <x:c r="L50" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M50" s="61" t="str">
+      <x:c r="M50" s="67" t="str">
         <x:v>Daily</x:v>
       </x:c>
-      <x:c r="N50" s="61" t="n">
+      <x:c r="N50" s="67" t="n">
         <x:v>276</x:v>
       </x:c>
-      <x:c r="O50" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P50" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q50" s="63" t="d">
+      <x:c r="O50" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P50" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q50" s="69" t="d">
         <x:v>2016-09-06T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R50" s="63" t="d">
+      <x:c r="R50" s="69" t="d">
         <x:v>2046-10-10T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S50" s="61" t="str">
+      <x:c r="S50" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T50" s="61" t="str">
+      <x:c r="T50" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U50" s="61" t="n">
+      <x:c r="U50" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V50" s="61" t="str">
+      <x:c r="V50" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="51">
-      <x:c r="B51" s="61" t="str">
+      <x:c r="B51" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C51" s="61" t="str">
+      <x:c r="C51" s="67" t="str">
         <x:v>S31632</x:v>
       </x:c>
-      <x:c r="D51" s="61" t="str">
+      <x:c r="D51" s="67" t="str">
         <x:v>LAU LEI CHEONG</x:v>
       </x:c>
-      <x:c r="E51" s="61" t="str">
+      <x:c r="E51" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F51" s="61" t="str">
+      <x:c r="F51" s="67" t="str">
         <x:v>Personal Care Worker</x:v>
       </x:c>
-      <x:c r="G51" s="61" t="str">
+      <x:c r="G51" s="67" t="str">
         <x:v>PCW</x:v>
       </x:c>
-      <x:c r="H51" s="61" t="str">
+      <x:c r="H51" s="67" t="str">
         <x:v>護理員 Personal Care  Worker</x:v>
       </x:c>
-      <x:c r="I51" s="63" t="d">
+      <x:c r="I51" s="69" t="d">
         <x:v>2016-09-07T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J51" s="61" t="n">
-        <x:v>3.5464</x:v>
-      </x:c>
-      <x:c r="K51" s="61" t="str">
+      <x:c r="J51" s="67" t="n">
+        <x:v>3.5492</x:v>
+      </x:c>
+      <x:c r="K51" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L51" s="61" t="str">
+      <x:c r="L51" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M51" s="61" t="str">
+      <x:c r="M51" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N51" s="61" t="n">
+      <x:c r="N51" s="67" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="O51" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P51" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q51" s="63" t="d">
+      <x:c r="O51" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P51" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q51" s="69" t="d">
         <x:v>2016-09-07T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R51" s="63" t="d">
+      <x:c r="R51" s="69" t="d">
         <x:v>2045-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S51" s="61" t="str">
+      <x:c r="S51" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T51" s="61" t="str">
+      <x:c r="T51" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U51" s="61" t="n">
+      <x:c r="U51" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V51" s="61" t="str">
+      <x:c r="V51" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>
     <x:row r="52">
-      <x:c r="B52" s="61" t="str">
+      <x:c r="A52" s="67" t="str">
+        <x:v>_DATAEND</x:v>
+      </x:c>
+      <x:c r="B52" s="67" t="str">
         <x:v>Data World Solutions Ltd</x:v>
       </x:c>
-      <x:c r="C52" s="61" t="str">
+      <x:c r="C52" s="67" t="str">
         <x:v>S31639</x:v>
       </x:c>
-      <x:c r="D52" s="61" t="str">
+      <x:c r="D52" s="67" t="str">
         <x:v>WOO Tsz Ching</x:v>
       </x:c>
-      <x:c r="E52" s="61" t="str">
+      <x:c r="E52" s="67" t="str">
         <x:v>Unit A</x:v>
       </x:c>
-      <x:c r="F52" s="61" t="str">
+      <x:c r="F52" s="67" t="str">
         <x:v>TEMPORARY STAFF 臨時員工</x:v>
       </x:c>
-      <x:c r="G52" s="61" t="str">
+      <x:c r="G52" s="67" t="str">
         <x:v>RW</x:v>
       </x:c>
-      <x:c r="H52" s="61" t="str">
+      <x:c r="H52" s="67" t="str">
         <x:v>RELIEF WORKER 支援人員</x:v>
       </x:c>
-      <x:c r="I52" s="63" t="d">
+      <x:c r="I52" s="69" t="d">
         <x:v>2017-10-20T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="J52" s="61" t="n">
-        <x:v>2.429</x:v>
-      </x:c>
-      <x:c r="K52" s="61" t="str">
+      <x:c r="J52" s="67" t="n">
+        <x:v>2.4317</x:v>
+      </x:c>
+      <x:c r="K52" s="67" t="str">
         <x:v>AL0</x:v>
       </x:c>
-      <x:c r="L52" s="61" t="str">
+      <x:c r="L52" s="67" t="str">
         <x:v>Statutory Holiday</x:v>
       </x:c>
-      <x:c r="M52" s="61" t="str">
+      <x:c r="M52" s="67" t="str">
         <x:v>Hourly</x:v>
       </x:c>
-      <x:c r="N52" s="61" t="n">
+      <x:c r="N52" s="67" t="n">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="O52" s="61" t="n">
-        <x:v/>
-      </x:c>
-      <x:c r="P52" s="61" t="str">
-        <x:v/>
-      </x:c>
-      <x:c r="Q52" s="63" t="d">
+      <x:c r="O52" s="67" t="n">
+        <x:v/>
+      </x:c>
+      <x:c r="P52" s="67" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="Q52" s="69" t="d">
         <x:v>2017-10-20T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="R52" s="63" t="d">
+      <x:c r="R52" s="69" t="d">
         <x:v>2100-01-01T00:00:00.0000000</x:v>
       </x:c>
-      <x:c r="S52" s="61" t="str">
+      <x:c r="S52" s="67" t="str">
         <x:v>Active</x:v>
       </x:c>
-      <x:c r="T52" s="61" t="str">
+      <x:c r="T52" s="67" t="str">
         <x:v>Yes</x:v>
       </x:c>
-      <x:c r="U52" s="61" t="n">
+      <x:c r="U52" s="67" t="n">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="V52" s="61" t="str">
+      <x:c r="V52" s="67" t="str">
         <x:v>DWS - CWB</x:v>
       </x:c>
     </x:row>

</xml_diff>